<commit_message>
Fixed cumulative code, wrote a function which gets every player and puts it in a spreadsheet. We can move the numbers for 'cumulative cumulative' into this sheet, as well as percentile
</commit_message>
<xml_diff>
--- a/Resources/2018/Cumulative_games_solo2018.xlsx
+++ b/Resources/2018/Cumulative_games_solo2018.xlsx
@@ -1990,7 +1990,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>226.5</v>
+        <v>271.8</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1998,7 +1998,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>271.6</v>
+        <v>325.92</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -2006,7 +2006,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>497.04</v>
+        <v>596.4480000000001</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -2014,7 +2014,7 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>273.24</v>
+        <v>327.888</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -2022,7 +2022,7 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>136.74</v>
+        <v>164.088</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -2030,7 +2030,7 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>9.66</v>
+        <v>11.592</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -2038,7 +2038,7 @@
         <v>8</v>
       </c>
       <c r="B8">
-        <v>526.5</v>
+        <v>693</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -2046,7 +2046,7 @@
         <v>9</v>
       </c>
       <c r="B9">
-        <v>288</v>
+        <v>345.6</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -2054,7 +2054,7 @@
         <v>10</v>
       </c>
       <c r="B10">
-        <v>21.24</v>
+        <v>25.488</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -2062,7 +2062,7 @@
         <v>11</v>
       </c>
       <c r="B11">
-        <v>54.56</v>
+        <v>65.47199999999999</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -2070,7 +2070,7 @@
         <v>12</v>
       </c>
       <c r="B12">
-        <v>414</v>
+        <v>496.8</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -2078,7 +2078,7 @@
         <v>13</v>
       </c>
       <c r="B13">
-        <v>104.12</v>
+        <v>124.944</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -2086,7 +2086,7 @@
         <v>14</v>
       </c>
       <c r="B14">
-        <v>395.16</v>
+        <v>474.192</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -2094,7 +2094,7 @@
         <v>15</v>
       </c>
       <c r="B15">
-        <v>344.52</v>
+        <v>413.424</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -2102,7 +2102,7 @@
         <v>16</v>
       </c>
       <c r="B16">
-        <v>5.94</v>
+        <v>7.128</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -2110,7 +2110,7 @@
         <v>17</v>
       </c>
       <c r="B17">
-        <v>574.5</v>
+        <v>750.6</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -2118,7 +2118,7 @@
         <v>18</v>
       </c>
       <c r="B18">
-        <v>500.76</v>
+        <v>600.912</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -2126,7 +2126,7 @@
         <v>19</v>
       </c>
       <c r="B19">
-        <v>296</v>
+        <v>355.2</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -2134,7 +2134,7 @@
         <v>20</v>
       </c>
       <c r="B20">
-        <v>60.96</v>
+        <v>73.15199999999999</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -2142,7 +2142,7 @@
         <v>21</v>
       </c>
       <c r="B21">
-        <v>454.2599999999999</v>
+        <v>545.112</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -2150,7 +2150,7 @@
         <v>22</v>
       </c>
       <c r="B22">
-        <v>28.12</v>
+        <v>33.744</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -2158,7 +2158,7 @@
         <v>23</v>
       </c>
       <c r="B23">
-        <v>55.8</v>
+        <v>66.95999999999999</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -2166,7 +2166,7 @@
         <v>24</v>
       </c>
       <c r="B24">
-        <v>36.36</v>
+        <v>43.63199999999999</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -2174,7 +2174,7 @@
         <v>25</v>
       </c>
       <c r="B25">
-        <v>352.4999999999999</v>
+        <v>423</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -2182,7 +2182,7 @@
         <v>26</v>
       </c>
       <c r="B26">
-        <v>143</v>
+        <v>171.6</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -2190,7 +2190,7 @@
         <v>27</v>
       </c>
       <c r="B27">
-        <v>143.1</v>
+        <v>171.72</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -2198,7 +2198,7 @@
         <v>28</v>
       </c>
       <c r="B28">
-        <v>77.14</v>
+        <v>92.56800000000001</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -2206,7 +2206,7 @@
         <v>29</v>
       </c>
       <c r="B29">
-        <v>15.96</v>
+        <v>19.152</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -2214,7 +2214,7 @@
         <v>30</v>
       </c>
       <c r="B30">
-        <v>361.68</v>
+        <v>438.816</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -2222,7 +2222,7 @@
         <v>31</v>
       </c>
       <c r="B31">
-        <v>320.16</v>
+        <v>384.192</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -2230,7 +2230,7 @@
         <v>32</v>
       </c>
       <c r="B32">
-        <v>526.6799999999999</v>
+        <v>632.016</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -2238,7 +2238,7 @@
         <v>33</v>
       </c>
       <c r="B33">
-        <v>536.22</v>
+        <v>643.4639999999999</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -2246,7 +2246,7 @@
         <v>34</v>
       </c>
       <c r="B34">
-        <v>396.8</v>
+        <v>476.16</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -2254,7 +2254,7 @@
         <v>35</v>
       </c>
       <c r="B35">
-        <v>184.86</v>
+        <v>221.832</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -2262,7 +2262,7 @@
         <v>36</v>
       </c>
       <c r="B36">
-        <v>296.46</v>
+        <v>355.752</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -2270,7 +2270,7 @@
         <v>37</v>
       </c>
       <c r="B37">
-        <v>357.4999999999999</v>
+        <v>429</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -2278,7 +2278,7 @@
         <v>38</v>
       </c>
       <c r="B38">
-        <v>595.3199999999999</v>
+        <v>714.3839999999999</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -2286,7 +2286,7 @@
         <v>39</v>
       </c>
       <c r="B39">
-        <v>116.56</v>
+        <v>139.872</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -2294,7 +2294,7 @@
         <v>40</v>
       </c>
       <c r="B40">
-        <v>330.04</v>
+        <v>396.048</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -2302,7 +2302,7 @@
         <v>41</v>
       </c>
       <c r="B41">
-        <v>388.8</v>
+        <v>466.56</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -2310,7 +2310,7 @@
         <v>42</v>
       </c>
       <c r="B42">
-        <v>161.88</v>
+        <v>194.256</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -2318,7 +2318,7 @@
         <v>43</v>
       </c>
       <c r="B43">
-        <v>90.99999999999999</v>
+        <v>109.2</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -2326,7 +2326,7 @@
         <v>44</v>
       </c>
       <c r="B44">
-        <v>413.28</v>
+        <v>495.936</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -2334,7 +2334,7 @@
         <v>45</v>
       </c>
       <c r="B45">
-        <v>217.14</v>
+        <v>260.568</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -2342,7 +2342,7 @@
         <v>46</v>
       </c>
       <c r="B46">
-        <v>66.88</v>
+        <v>80.25599999999999</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -2350,7 +2350,7 @@
         <v>47</v>
       </c>
       <c r="B47">
-        <v>115.92</v>
+        <v>139.104</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -2358,7 +2358,7 @@
         <v>48</v>
       </c>
       <c r="B48">
-        <v>22.88</v>
+        <v>27.456</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -2366,7 +2366,7 @@
         <v>49</v>
       </c>
       <c r="B49">
-        <v>298.48</v>
+        <v>358.1759999999999</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -2374,7 +2374,7 @@
         <v>50</v>
       </c>
       <c r="B50">
-        <v>274.7</v>
+        <v>329.64</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -2382,7 +2382,7 @@
         <v>51</v>
       </c>
       <c r="B51">
-        <v>107.1</v>
+        <v>128.52</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -2390,7 +2390,7 @@
         <v>52</v>
       </c>
       <c r="B52">
-        <v>62.7</v>
+        <v>75.23999999999999</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -2398,7 +2398,7 @@
         <v>53</v>
       </c>
       <c r="B53">
-        <v>464.72</v>
+        <v>557.664</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -2406,7 +2406,7 @@
         <v>54</v>
       </c>
       <c r="B54">
-        <v>9</v>
+        <v>10.8</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -2414,7 +2414,7 @@
         <v>55</v>
       </c>
       <c r="B55">
-        <v>441.24</v>
+        <v>534.2879999999999</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -2422,7 +2422,7 @@
         <v>56</v>
       </c>
       <c r="B56">
-        <v>492.8</v>
+        <v>591.36</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -2430,7 +2430,7 @@
         <v>57</v>
       </c>
       <c r="B57">
-        <v>43.23999999999999</v>
+        <v>51.88800000000001</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -2438,7 +2438,7 @@
         <v>58</v>
       </c>
       <c r="B58">
-        <v>7.56</v>
+        <v>9.071999999999999</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -2446,7 +2446,7 @@
         <v>59</v>
       </c>
       <c r="B59">
-        <v>372.6</v>
+        <v>447.12</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -2454,7 +2454,7 @@
         <v>60</v>
       </c>
       <c r="B60">
-        <v>231.2</v>
+        <v>277.44</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -2462,7 +2462,7 @@
         <v>61</v>
       </c>
       <c r="B61">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -2470,7 +2470,7 @@
         <v>62</v>
       </c>
       <c r="B62">
-        <v>287.04</v>
+        <v>344.448</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -2478,7 +2478,7 @@
         <v>63</v>
       </c>
       <c r="B63">
-        <v>5.76</v>
+        <v>6.912</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -2486,7 +2486,7 @@
         <v>64</v>
       </c>
       <c r="B64">
-        <v>241.92</v>
+        <v>290.304</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -2494,7 +2494,7 @@
         <v>65</v>
       </c>
       <c r="B65">
-        <v>287.04</v>
+        <v>344.4479999999999</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -2502,7 +2502,7 @@
         <v>66</v>
       </c>
       <c r="B66">
-        <v>37.76</v>
+        <v>45.312</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -2510,7 +2510,7 @@
         <v>67</v>
       </c>
       <c r="B67">
-        <v>470.6799999999999</v>
+        <v>564.816</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -2518,7 +2518,7 @@
         <v>68</v>
       </c>
       <c r="B68">
-        <v>38.64</v>
+        <v>46.368</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -2526,7 +2526,7 @@
         <v>69</v>
       </c>
       <c r="B69">
-        <v>0.7999999999999999</v>
+        <v>0.96</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -2534,7 +2534,7 @@
         <v>70</v>
       </c>
       <c r="B70">
-        <v>23.2</v>
+        <v>27.84</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -2542,7 +2542,7 @@
         <v>71</v>
       </c>
       <c r="B71">
-        <v>429.8</v>
+        <v>515.76</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -2550,7 +2550,7 @@
         <v>72</v>
       </c>
       <c r="B72">
-        <v>27.72</v>
+        <v>33.264</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -2558,7 +2558,7 @@
         <v>73</v>
       </c>
       <c r="B73">
-        <v>6.24</v>
+        <v>7.488</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -2566,7 +2566,7 @@
         <v>74</v>
       </c>
       <c r="B74">
-        <v>155.52</v>
+        <v>186.624</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -2574,7 +2574,7 @@
         <v>75</v>
       </c>
       <c r="B75">
-        <v>2</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -2582,7 +2582,7 @@
         <v>76</v>
       </c>
       <c r="B76">
-        <v>14.4</v>
+        <v>17.28</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -2590,7 +2590,7 @@
         <v>77</v>
       </c>
       <c r="B77">
-        <v>345.9599999999999</v>
+        <v>415.152</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -2598,7 +2598,7 @@
         <v>78</v>
       </c>
       <c r="B78">
-        <v>156.96</v>
+        <v>188.352</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -2606,7 +2606,7 @@
         <v>79</v>
       </c>
       <c r="B79">
-        <v>211.2</v>
+        <v>253.44</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -2614,7 +2614,7 @@
         <v>80</v>
       </c>
       <c r="B80">
-        <v>493.06</v>
+        <v>699.672</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -2622,7 +2622,7 @@
         <v>81</v>
       </c>
       <c r="B81">
-        <v>85.25999999999999</v>
+        <v>102.312</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -2630,7 +2630,7 @@
         <v>82</v>
       </c>
       <c r="B82">
-        <v>21.36</v>
+        <v>25.632</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -2638,7 +2638,7 @@
         <v>83</v>
       </c>
       <c r="B83">
-        <v>182.4</v>
+        <v>218.88</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -2646,7 +2646,7 @@
         <v>84</v>
       </c>
       <c r="B84">
-        <v>491.36</v>
+        <v>589.6320000000001</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -2654,7 +2654,7 @@
         <v>85</v>
       </c>
       <c r="B85">
-        <v>84.40000000000001</v>
+        <v>101.28</v>
       </c>
     </row>
     <row r="86" spans="1:2">
@@ -2662,7 +2662,7 @@
         <v>86</v>
       </c>
       <c r="B86">
-        <v>406.9999999999999</v>
+        <v>488.4</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -2670,7 +2670,7 @@
         <v>87</v>
       </c>
       <c r="B87">
-        <v>436.54</v>
+        <v>523.848</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -2678,7 +2678,7 @@
         <v>88</v>
       </c>
       <c r="B88">
-        <v>205.32</v>
+        <v>246.384</v>
       </c>
     </row>
     <row r="89" spans="1:2">
@@ -2686,7 +2686,7 @@
         <v>89</v>
       </c>
       <c r="B89">
-        <v>167.44</v>
+        <v>200.928</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -2694,7 +2694,7 @@
         <v>90</v>
       </c>
       <c r="B90">
-        <v>112.48</v>
+        <v>134.976</v>
       </c>
     </row>
     <row r="91" spans="1:2">
@@ -2702,7 +2702,7 @@
         <v>91</v>
       </c>
       <c r="B91">
-        <v>148.4</v>
+        <v>178.08</v>
       </c>
     </row>
     <row r="92" spans="1:2">
@@ -2710,7 +2710,7 @@
         <v>92</v>
       </c>
       <c r="B92">
-        <v>408.8</v>
+        <v>490.56</v>
       </c>
     </row>
     <row r="93" spans="1:2">
@@ -2718,7 +2718,7 @@
         <v>93</v>
       </c>
       <c r="B93">
-        <v>103.74</v>
+        <v>124.488</v>
       </c>
     </row>
     <row r="94" spans="1:2">
@@ -2726,7 +2726,7 @@
         <v>94</v>
       </c>
       <c r="B94">
-        <v>283.8</v>
+        <v>340.56</v>
       </c>
     </row>
     <row r="95" spans="1:2">
@@ -2734,7 +2734,7 @@
         <v>95</v>
       </c>
       <c r="B95">
-        <v>230</v>
+        <v>276</v>
       </c>
     </row>
     <row r="96" spans="1:2">
@@ -2742,7 +2742,7 @@
         <v>96</v>
       </c>
       <c r="B96">
-        <v>469.16</v>
+        <v>562.992</v>
       </c>
     </row>
     <row r="97" spans="1:2">
@@ -2750,7 +2750,7 @@
         <v>97</v>
       </c>
       <c r="B97">
-        <v>305.28</v>
+        <v>366.336</v>
       </c>
     </row>
     <row r="98" spans="1:2">
@@ -2758,7 +2758,7 @@
         <v>98</v>
       </c>
       <c r="B98">
-        <v>291.5599999999999</v>
+        <v>349.872</v>
       </c>
     </row>
     <row r="99" spans="1:2">
@@ -2766,7 +2766,7 @@
         <v>99</v>
       </c>
       <c r="B99">
-        <v>377.46</v>
+        <v>452.952</v>
       </c>
     </row>
     <row r="100" spans="1:2">
@@ -2774,7 +2774,7 @@
         <v>100</v>
       </c>
       <c r="B100">
-        <v>12.74</v>
+        <v>15.288</v>
       </c>
     </row>
     <row r="101" spans="1:2">
@@ -2782,7 +2782,7 @@
         <v>101</v>
       </c>
       <c r="B101">
-        <v>24.48</v>
+        <v>29.376</v>
       </c>
     </row>
     <row r="102" spans="1:2">
@@ -2790,7 +2790,7 @@
         <v>102</v>
       </c>
       <c r="B102">
-        <v>362.6799999999999</v>
+        <v>440.016</v>
       </c>
     </row>
     <row r="103" spans="1:2">
@@ -2798,7 +2798,7 @@
         <v>103</v>
       </c>
       <c r="B103">
-        <v>208.56</v>
+        <v>250.272</v>
       </c>
     </row>
     <row r="104" spans="1:2">
@@ -2806,7 +2806,7 @@
         <v>104</v>
       </c>
       <c r="B104">
-        <v>96</v>
+        <v>115.2</v>
       </c>
     </row>
     <row r="105" spans="1:2">
@@ -2814,7 +2814,7 @@
         <v>105</v>
       </c>
       <c r="B105">
-        <v>402.9599999999999</v>
+        <v>483.552</v>
       </c>
     </row>
     <row r="106" spans="1:2">
@@ -2822,7 +2822,7 @@
         <v>106</v>
       </c>
       <c r="B106">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="107" spans="1:2">
@@ -2830,7 +2830,7 @@
         <v>107</v>
       </c>
       <c r="B107">
-        <v>74.64</v>
+        <v>89.56800000000001</v>
       </c>
     </row>
     <row r="108" spans="1:2">
@@ -2838,7 +2838,7 @@
         <v>108</v>
       </c>
       <c r="B108">
-        <v>296.84</v>
+        <v>356.208</v>
       </c>
     </row>
     <row r="109" spans="1:2">
@@ -2846,7 +2846,7 @@
         <v>109</v>
       </c>
       <c r="B109">
-        <v>147.84</v>
+        <v>177.408</v>
       </c>
     </row>
     <row r="110" spans="1:2">
@@ -2854,7 +2854,7 @@
         <v>110</v>
       </c>
       <c r="B110">
-        <v>7.539999999999999</v>
+        <v>9.047999999999998</v>
       </c>
     </row>
     <row r="111" spans="1:2">
@@ -2862,7 +2862,7 @@
         <v>111</v>
       </c>
       <c r="B111">
-        <v>17.36</v>
+        <v>20.832</v>
       </c>
     </row>
     <row r="112" spans="1:2">
@@ -2870,7 +2870,7 @@
         <v>112</v>
       </c>
       <c r="B112">
-        <v>6.399999999999999</v>
+        <v>7.68</v>
       </c>
     </row>
     <row r="113" spans="1:2">
@@ -2878,7 +2878,7 @@
         <v>113</v>
       </c>
       <c r="B113">
-        <v>347.52</v>
+        <v>417.024</v>
       </c>
     </row>
     <row r="114" spans="1:2">
@@ -2886,7 +2886,7 @@
         <v>114</v>
       </c>
       <c r="B114">
-        <v>543.2</v>
+        <v>698.64</v>
       </c>
     </row>
     <row r="115" spans="1:2">
@@ -2894,7 +2894,7 @@
         <v>115</v>
       </c>
       <c r="B115">
-        <v>439.5</v>
+        <v>527.4</v>
       </c>
     </row>
     <row r="116" spans="1:2">
@@ -2902,7 +2902,7 @@
         <v>116</v>
       </c>
       <c r="B116">
-        <v>125.58</v>
+        <v>150.696</v>
       </c>
     </row>
     <row r="117" spans="1:2">
@@ -2910,7 +2910,7 @@
         <v>117</v>
       </c>
       <c r="B117">
-        <v>331.2</v>
+        <v>397.44</v>
       </c>
     </row>
     <row r="118" spans="1:2">
@@ -2918,7 +2918,7 @@
         <v>118</v>
       </c>
       <c r="B118">
-        <v>10.6</v>
+        <v>12.72</v>
       </c>
     </row>
     <row r="119" spans="1:2">
@@ -2926,7 +2926,7 @@
         <v>119</v>
       </c>
       <c r="B119">
-        <v>417.6</v>
+        <v>501.12</v>
       </c>
     </row>
     <row r="120" spans="1:2">
@@ -2934,7 +2934,7 @@
         <v>120</v>
       </c>
       <c r="B120">
-        <v>312.4399999999999</v>
+        <v>374.9279999999999</v>
       </c>
     </row>
     <row r="121" spans="1:2">
@@ -2942,7 +2942,7 @@
         <v>121</v>
       </c>
       <c r="B121">
-        <v>350.4</v>
+        <v>481.68</v>
       </c>
     </row>
     <row r="122" spans="1:2">
@@ -2950,7 +2950,7 @@
         <v>122</v>
       </c>
       <c r="B122">
-        <v>323.9</v>
+        <v>388.68</v>
       </c>
     </row>
     <row r="123" spans="1:2">
@@ -2958,7 +2958,7 @@
         <v>123</v>
       </c>
       <c r="B123">
-        <v>606</v>
+        <v>835.1999999999999</v>
       </c>
     </row>
     <row r="124" spans="1:2">
@@ -2966,7 +2966,7 @@
         <v>124</v>
       </c>
       <c r="B124">
-        <v>188.48</v>
+        <v>226.176</v>
       </c>
     </row>
     <row r="125" spans="1:2">
@@ -2974,7 +2974,7 @@
         <v>125</v>
       </c>
       <c r="B125">
-        <v>294.84</v>
+        <v>353.8079999999999</v>
       </c>
     </row>
     <row r="126" spans="1:2">
@@ -2982,7 +2982,7 @@
         <v>126</v>
       </c>
       <c r="B126">
-        <v>308.76</v>
+        <v>370.512</v>
       </c>
     </row>
     <row r="127" spans="1:2">
@@ -2990,7 +2990,7 @@
         <v>127</v>
       </c>
       <c r="B127">
-        <v>176.66</v>
+        <v>211.992</v>
       </c>
     </row>
     <row r="128" spans="1:2">
@@ -2998,7 +2998,7 @@
         <v>128</v>
       </c>
       <c r="B128">
-        <v>203.04</v>
+        <v>243.648</v>
       </c>
     </row>
     <row r="129" spans="1:2">
@@ -3006,7 +3006,7 @@
         <v>129</v>
       </c>
       <c r="B129">
-        <v>142.12</v>
+        <v>170.544</v>
       </c>
     </row>
     <row r="130" spans="1:2">
@@ -3014,7 +3014,7 @@
         <v>130</v>
       </c>
       <c r="B130">
-        <v>2.6</v>
+        <v>3.12</v>
       </c>
     </row>
     <row r="131" spans="1:2">
@@ -3022,7 +3022,7 @@
         <v>131</v>
       </c>
       <c r="B131">
-        <v>566.4</v>
+        <v>740.88</v>
       </c>
     </row>
     <row r="132" spans="1:2">
@@ -3030,7 +3030,7 @@
         <v>132</v>
       </c>
       <c r="B132">
-        <v>116.48</v>
+        <v>139.776</v>
       </c>
     </row>
     <row r="133" spans="1:2">
@@ -3038,7 +3038,7 @@
         <v>133</v>
       </c>
       <c r="B133">
-        <v>267.02</v>
+        <v>320.424</v>
       </c>
     </row>
     <row r="134" spans="1:2">
@@ -3046,7 +3046,7 @@
         <v>134</v>
       </c>
       <c r="B134">
-        <v>460.8</v>
+        <v>552.96</v>
       </c>
     </row>
     <row r="135" spans="1:2">
@@ -3054,7 +3054,7 @@
         <v>135</v>
       </c>
       <c r="B135">
-        <v>194.88</v>
+        <v>233.856</v>
       </c>
     </row>
     <row r="136" spans="1:2">
@@ -3062,7 +3062,7 @@
         <v>136</v>
       </c>
       <c r="B136">
-        <v>95.04000000000001</v>
+        <v>114.048</v>
       </c>
     </row>
     <row r="137" spans="1:2">
@@ -3070,7 +3070,7 @@
         <v>137</v>
       </c>
       <c r="B137">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="138" spans="1:2">
@@ -3078,7 +3078,7 @@
         <v>138</v>
       </c>
       <c r="B138">
-        <v>0.6</v>
+        <v>0.72</v>
       </c>
     </row>
     <row r="139" spans="1:2">
@@ -3086,7 +3086,7 @@
         <v>139</v>
       </c>
       <c r="B139">
-        <v>475.5</v>
+        <v>570.6</v>
       </c>
     </row>
     <row r="140" spans="1:2">
@@ -3094,7 +3094,7 @@
         <v>140</v>
       </c>
       <c r="B140">
-        <v>14</v>
+        <v>16.8</v>
       </c>
     </row>
     <row r="141" spans="1:2">
@@ -3102,7 +3102,7 @@
         <v>141</v>
       </c>
       <c r="B141">
-        <v>525.72</v>
+        <v>630.864</v>
       </c>
     </row>
     <row r="142" spans="1:2">
@@ -3110,7 +3110,7 @@
         <v>142</v>
       </c>
       <c r="B142">
-        <v>137.28</v>
+        <v>164.736</v>
       </c>
     </row>
     <row r="143" spans="1:2">
@@ -3118,7 +3118,7 @@
         <v>143</v>
       </c>
       <c r="B143">
-        <v>304.72</v>
+        <v>365.664</v>
       </c>
     </row>
     <row r="144" spans="1:2">
@@ -3126,7 +3126,7 @@
         <v>144</v>
       </c>
       <c r="B144">
-        <v>489.12</v>
+        <v>648.1440000000001</v>
       </c>
     </row>
     <row r="145" spans="1:2">
@@ -3134,7 +3134,7 @@
         <v>145</v>
       </c>
       <c r="B145">
-        <v>1.8</v>
+        <v>2.16</v>
       </c>
     </row>
     <row r="146" spans="1:2">
@@ -3142,7 +3142,7 @@
         <v>146</v>
       </c>
       <c r="B146">
-        <v>66.12</v>
+        <v>79.34399999999999</v>
       </c>
     </row>
     <row r="147" spans="1:2">
@@ -3150,7 +3150,7 @@
         <v>147</v>
       </c>
       <c r="B147">
-        <v>408.1</v>
+        <v>489.72</v>
       </c>
     </row>
     <row r="148" spans="1:2">
@@ -3158,7 +3158,7 @@
         <v>148</v>
       </c>
       <c r="B148">
-        <v>441.78</v>
+        <v>638.136</v>
       </c>
     </row>
     <row r="149" spans="1:2">
@@ -3166,7 +3166,7 @@
         <v>149</v>
       </c>
       <c r="B149">
-        <v>321.12</v>
+        <v>385.344</v>
       </c>
     </row>
     <row r="150" spans="1:2">
@@ -3174,7 +3174,7 @@
         <v>150</v>
       </c>
       <c r="B150">
-        <v>136.08</v>
+        <v>163.296</v>
       </c>
     </row>
     <row r="151" spans="1:2">
@@ -3182,7 +3182,7 @@
         <v>151</v>
       </c>
       <c r="B151">
-        <v>155.52</v>
+        <v>186.624</v>
       </c>
     </row>
     <row r="152" spans="1:2">
@@ -3190,7 +3190,7 @@
         <v>152</v>
       </c>
       <c r="B152">
-        <v>1</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="153" spans="1:2">
@@ -3198,7 +3198,7 @@
         <v>153</v>
       </c>
       <c r="B153">
-        <v>321.36</v>
+        <v>385.6319999999999</v>
       </c>
     </row>
     <row r="154" spans="1:2">
@@ -3206,7 +3206,7 @@
         <v>154</v>
       </c>
       <c r="B154">
-        <v>47.04000000000001</v>
+        <v>56.448</v>
       </c>
     </row>
     <row r="155" spans="1:2">
@@ -3214,7 +3214,7 @@
         <v>155</v>
       </c>
       <c r="B155">
-        <v>92.16</v>
+        <v>110.592</v>
       </c>
     </row>
     <row r="156" spans="1:2">
@@ -3222,7 +3222,7 @@
         <v>156</v>
       </c>
       <c r="B156">
-        <v>431.2</v>
+        <v>517.4399999999999</v>
       </c>
     </row>
     <row r="157" spans="1:2">
@@ -3230,7 +3230,7 @@
         <v>157</v>
       </c>
       <c r="B157">
-        <v>28.16</v>
+        <v>33.792</v>
       </c>
     </row>
     <row r="158" spans="1:2">
@@ -3238,7 +3238,7 @@
         <v>158</v>
       </c>
       <c r="B158">
-        <v>195.8</v>
+        <v>234.96</v>
       </c>
     </row>
     <row r="159" spans="1:2">
@@ -3246,7 +3246,7 @@
         <v>159</v>
       </c>
       <c r="B159">
-        <v>272.24</v>
+        <v>326.688</v>
       </c>
     </row>
     <row r="160" spans="1:2">
@@ -3254,7 +3254,7 @@
         <v>160</v>
       </c>
       <c r="B160">
-        <v>152.5</v>
+        <v>183</v>
       </c>
     </row>
     <row r="161" spans="1:2">
@@ -3262,7 +3262,7 @@
         <v>161</v>
       </c>
       <c r="B161">
-        <v>455.92</v>
+        <v>547.1039999999999</v>
       </c>
     </row>
     <row r="162" spans="1:2">
@@ -3270,7 +3270,7 @@
         <v>162</v>
       </c>
       <c r="B162">
-        <v>89.45999999999999</v>
+        <v>107.352</v>
       </c>
     </row>
     <row r="163" spans="1:2">
@@ -3278,7 +3278,7 @@
         <v>163</v>
       </c>
       <c r="B163">
-        <v>304</v>
+        <v>364.8</v>
       </c>
     </row>
     <row r="164" spans="1:2">
@@ -3286,7 +3286,7 @@
         <v>164</v>
       </c>
       <c r="B164">
-        <v>367.08</v>
+        <v>440.496</v>
       </c>
     </row>
     <row r="165" spans="1:2">
@@ -3294,7 +3294,7 @@
         <v>165</v>
       </c>
       <c r="B165">
-        <v>405.8800000000001</v>
+        <v>487.056</v>
       </c>
     </row>
     <row r="166" spans="1:2">
@@ -3302,7 +3302,7 @@
         <v>166</v>
       </c>
       <c r="B166">
-        <v>167.56</v>
+        <v>201.072</v>
       </c>
     </row>
     <row r="167" spans="1:2">
@@ -3310,7 +3310,7 @@
         <v>167</v>
       </c>
       <c r="B167">
-        <v>138.86</v>
+        <v>166.632</v>
       </c>
     </row>
     <row r="168" spans="1:2">
@@ -3318,7 +3318,7 @@
         <v>168</v>
       </c>
       <c r="B168">
-        <v>50.68</v>
+        <v>60.816</v>
       </c>
     </row>
     <row r="169" spans="1:2">
@@ -3326,7 +3326,7 @@
         <v>169</v>
       </c>
       <c r="B169">
-        <v>134.4</v>
+        <v>161.28</v>
       </c>
     </row>
     <row r="170" spans="1:2">
@@ -3334,7 +3334,7 @@
         <v>170</v>
       </c>
       <c r="B170">
-        <v>172.84</v>
+        <v>207.408</v>
       </c>
     </row>
     <row r="171" spans="1:2">
@@ -3342,7 +3342,7 @@
         <v>171</v>
       </c>
       <c r="B171">
-        <v>481.8</v>
+        <v>578.16</v>
       </c>
     </row>
     <row r="172" spans="1:2">
@@ -3350,7 +3350,7 @@
         <v>172</v>
       </c>
       <c r="B172">
-        <v>361.8999999999999</v>
+        <v>434.28</v>
       </c>
     </row>
     <row r="173" spans="1:2">
@@ -3358,7 +3358,7 @@
         <v>173</v>
       </c>
       <c r="B173">
-        <v>246.24</v>
+        <v>295.488</v>
       </c>
     </row>
     <row r="174" spans="1:2">
@@ -3366,7 +3366,7 @@
         <v>174</v>
       </c>
       <c r="B174">
-        <v>602.28</v>
+        <v>783.936</v>
       </c>
     </row>
     <row r="175" spans="1:2">
@@ -3374,7 +3374,7 @@
         <v>175</v>
       </c>
       <c r="B175">
-        <v>44.52</v>
+        <v>53.424</v>
       </c>
     </row>
     <row r="176" spans="1:2">
@@ -3382,7 +3382,7 @@
         <v>176</v>
       </c>
       <c r="B176">
-        <v>8</v>
+        <v>9.6</v>
       </c>
     </row>
     <row r="177" spans="1:2">
@@ -3390,7 +3390,7 @@
         <v>177</v>
       </c>
       <c r="B177">
-        <v>544.48</v>
+        <v>653.376</v>
       </c>
     </row>
     <row r="178" spans="1:2">
@@ -3398,7 +3398,7 @@
         <v>178</v>
       </c>
       <c r="B178">
-        <v>260</v>
+        <v>312</v>
       </c>
     </row>
     <row r="179" spans="1:2">
@@ -3406,7 +3406,7 @@
         <v>179</v>
       </c>
       <c r="B179">
-        <v>758.88</v>
+        <v>975.4559999999999</v>
       </c>
     </row>
     <row r="180" spans="1:2">
@@ -3414,7 +3414,7 @@
         <v>180</v>
       </c>
       <c r="B180">
-        <v>381.64</v>
+        <v>457.968</v>
       </c>
     </row>
     <row r="181" spans="1:2">
@@ -3422,7 +3422,7 @@
         <v>181</v>
       </c>
       <c r="B181">
-        <v>430.56</v>
+        <v>516.6719999999999</v>
       </c>
     </row>
     <row r="182" spans="1:2">
@@ -3430,7 +3430,7 @@
         <v>182</v>
       </c>
       <c r="B182">
-        <v>414.92</v>
+        <v>497.9039999999999</v>
       </c>
     </row>
     <row r="183" spans="1:2">
@@ -3438,7 +3438,7 @@
         <v>183</v>
       </c>
       <c r="B183">
-        <v>210.42</v>
+        <v>252.504</v>
       </c>
     </row>
     <row r="184" spans="1:2">
@@ -3446,7 +3446,7 @@
         <v>184</v>
       </c>
       <c r="B184">
-        <v>328.86</v>
+        <v>394.6319999999999</v>
       </c>
     </row>
     <row r="185" spans="1:2">
@@ -3454,7 +3454,7 @@
         <v>185</v>
       </c>
       <c r="B185">
-        <v>337.4400000000001</v>
+        <v>404.928</v>
       </c>
     </row>
     <row r="186" spans="1:2">
@@ -3462,7 +3462,7 @@
         <v>186</v>
       </c>
       <c r="B186">
-        <v>17.2</v>
+        <v>20.64</v>
       </c>
     </row>
     <row r="187" spans="1:2">
@@ -3470,7 +3470,7 @@
         <v>187</v>
       </c>
       <c r="B187">
-        <v>358.4</v>
+        <v>430.08</v>
       </c>
     </row>
     <row r="188" spans="1:2">
@@ -3478,7 +3478,7 @@
         <v>188</v>
       </c>
       <c r="B188">
-        <v>493.8</v>
+        <v>639.36</v>
       </c>
     </row>
     <row r="189" spans="1:2">
@@ -3486,7 +3486,7 @@
         <v>189</v>
       </c>
       <c r="B189">
-        <v>186.14</v>
+        <v>223.368</v>
       </c>
     </row>
     <row r="190" spans="1:2">
@@ -3494,7 +3494,7 @@
         <v>190</v>
       </c>
       <c r="B190">
-        <v>308.0000000000001</v>
+        <v>369.6</v>
       </c>
     </row>
     <row r="191" spans="1:2">
@@ -3502,7 +3502,7 @@
         <v>191</v>
       </c>
       <c r="B191">
-        <v>365.04</v>
+        <v>438.0479999999999</v>
       </c>
     </row>
     <row r="192" spans="1:2">
@@ -3510,7 +3510,7 @@
         <v>192</v>
       </c>
       <c r="B192">
-        <v>394.4</v>
+        <v>473.28</v>
       </c>
     </row>
     <row r="193" spans="1:2">
@@ -3518,7 +3518,7 @@
         <v>193</v>
       </c>
       <c r="B193">
-        <v>5.64</v>
+        <v>6.768000000000001</v>
       </c>
     </row>
     <row r="194" spans="1:2">
@@ -3526,7 +3526,7 @@
         <v>194</v>
       </c>
       <c r="B194">
-        <v>377.34</v>
+        <v>452.808</v>
       </c>
     </row>
     <row r="195" spans="1:2">
@@ -3534,7 +3534,7 @@
         <v>195</v>
       </c>
       <c r="B195">
-        <v>893.76</v>
+        <v>1151.712</v>
       </c>
     </row>
     <row r="196" spans="1:2">
@@ -3542,7 +3542,7 @@
         <v>196</v>
       </c>
       <c r="B196">
-        <v>252.52</v>
+        <v>303.0239999999999</v>
       </c>
     </row>
     <row r="197" spans="1:2">
@@ -3550,7 +3550,7 @@
         <v>197</v>
       </c>
       <c r="B197">
-        <v>258.4</v>
+        <v>310.08</v>
       </c>
     </row>
     <row r="198" spans="1:2">
@@ -3558,7 +3558,7 @@
         <v>198</v>
       </c>
       <c r="B198">
-        <v>268.38</v>
+        <v>322.056</v>
       </c>
     </row>
     <row r="199" spans="1:2">
@@ -3566,7 +3566,7 @@
         <v>199</v>
       </c>
       <c r="B199">
-        <v>460.96</v>
+        <v>553.1519999999999</v>
       </c>
     </row>
     <row r="200" spans="1:2">
@@ -3574,7 +3574,7 @@
         <v>200</v>
       </c>
       <c r="B200">
-        <v>394.6799999999999</v>
+        <v>473.616</v>
       </c>
     </row>
     <row r="201" spans="1:2">
@@ -3582,7 +3582,7 @@
         <v>201</v>
       </c>
       <c r="B201">
-        <v>534.4</v>
+        <v>641.28</v>
       </c>
     </row>
     <row r="202" spans="1:2">
@@ -3590,7 +3590,7 @@
         <v>202</v>
       </c>
       <c r="B202">
-        <v>46.62</v>
+        <v>55.944</v>
       </c>
     </row>
     <row r="203" spans="1:2">
@@ -3598,7 +3598,7 @@
         <v>203</v>
       </c>
       <c r="B203">
-        <v>265.4399999999999</v>
+        <v>318.528</v>
       </c>
     </row>
     <row r="204" spans="1:2">
@@ -3606,7 +3606,7 @@
         <v>204</v>
       </c>
       <c r="B204">
-        <v>76.81999999999999</v>
+        <v>92.18399999999998</v>
       </c>
     </row>
     <row r="205" spans="1:2">
@@ -3614,7 +3614,7 @@
         <v>205</v>
       </c>
       <c r="B205">
-        <v>292.32</v>
+        <v>350.784</v>
       </c>
     </row>
     <row r="206" spans="1:2">
@@ -3622,7 +3622,7 @@
         <v>206</v>
       </c>
       <c r="B206">
-        <v>14.28</v>
+        <v>17.136</v>
       </c>
     </row>
     <row r="207" spans="1:2">
@@ -3630,7 +3630,7 @@
         <v>207</v>
       </c>
       <c r="B207">
-        <v>24.48</v>
+        <v>29.376</v>
       </c>
     </row>
     <row r="208" spans="1:2">
@@ -3638,7 +3638,7 @@
         <v>208</v>
       </c>
       <c r="B208">
-        <v>1</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="209" spans="1:2">
@@ -3646,7 +3646,7 @@
         <v>209</v>
       </c>
       <c r="B209">
-        <v>1.38</v>
+        <v>1.656</v>
       </c>
     </row>
     <row r="210" spans="1:2">
@@ -3654,7 +3654,7 @@
         <v>210</v>
       </c>
       <c r="B210">
-        <v>75.59999999999999</v>
+        <v>90.72</v>
       </c>
     </row>
     <row r="211" spans="1:2">
@@ -3662,7 +3662,7 @@
         <v>211</v>
       </c>
       <c r="B211">
-        <v>393.6799999999999</v>
+        <v>472.4159999999999</v>
       </c>
     </row>
     <row r="212" spans="1:2">
@@ -3670,7 +3670,7 @@
         <v>212</v>
       </c>
       <c r="B212">
-        <v>55.49999999999999</v>
+        <v>66.59999999999999</v>
       </c>
     </row>
     <row r="213" spans="1:2">
@@ -3678,7 +3678,7 @@
         <v>213</v>
       </c>
       <c r="B213">
-        <v>98.88</v>
+        <v>118.656</v>
       </c>
     </row>
     <row r="214" spans="1:2">
@@ -3686,7 +3686,7 @@
         <v>214</v>
       </c>
       <c r="B214">
-        <v>331.5</v>
+        <v>397.8</v>
       </c>
     </row>
     <row r="215" spans="1:2">
@@ -3694,7 +3694,7 @@
         <v>215</v>
       </c>
       <c r="B215">
-        <v>47.88</v>
+        <v>57.456</v>
       </c>
     </row>
     <row r="216" spans="1:2">
@@ -3702,7 +3702,7 @@
         <v>216</v>
       </c>
       <c r="B216">
-        <v>404.8</v>
+        <v>485.76</v>
       </c>
     </row>
     <row r="217" spans="1:2">
@@ -3710,7 +3710,7 @@
         <v>217</v>
       </c>
       <c r="B217">
-        <v>151.84</v>
+        <v>182.208</v>
       </c>
     </row>
     <row r="218" spans="1:2">
@@ -3718,7 +3718,7 @@
         <v>218</v>
       </c>
       <c r="B218">
-        <v>361.8</v>
+        <v>434.16</v>
       </c>
     </row>
     <row r="219" spans="1:2">
@@ -3726,7 +3726,7 @@
         <v>219</v>
       </c>
       <c r="B219">
-        <v>37.44</v>
+        <v>44.928</v>
       </c>
     </row>
     <row r="220" spans="1:2">
@@ -3734,7 +3734,7 @@
         <v>220</v>
       </c>
       <c r="B220">
-        <v>19.04</v>
+        <v>22.848</v>
       </c>
     </row>
     <row r="221" spans="1:2">
@@ -3742,7 +3742,7 @@
         <v>221</v>
       </c>
       <c r="B221">
-        <v>620.8199999999999</v>
+        <v>791.784</v>
       </c>
     </row>
     <row r="222" spans="1:2">
@@ -3750,7 +3750,7 @@
         <v>222</v>
       </c>
       <c r="B222">
-        <v>453.6</v>
+        <v>544.3199999999999</v>
       </c>
     </row>
     <row r="223" spans="1:2">
@@ -3758,7 +3758,7 @@
         <v>223</v>
       </c>
       <c r="B223">
-        <v>35.03999999999999</v>
+        <v>42.04799999999999</v>
       </c>
     </row>
     <row r="224" spans="1:2">
@@ -3766,7 +3766,7 @@
         <v>224</v>
       </c>
       <c r="B224">
-        <v>383.52</v>
+        <v>460.224</v>
       </c>
     </row>
     <row r="225" spans="1:2">
@@ -3774,7 +3774,7 @@
         <v>225</v>
       </c>
       <c r="B225">
-        <v>148.8</v>
+        <v>178.56</v>
       </c>
     </row>
     <row r="226" spans="1:2">
@@ -3782,7 +3782,7 @@
         <v>226</v>
       </c>
       <c r="B226">
-        <v>322.8</v>
+        <v>387.36</v>
       </c>
     </row>
     <row r="227" spans="1:2">
@@ -3790,7 +3790,7 @@
         <v>227</v>
       </c>
       <c r="B227">
-        <v>1.6</v>
+        <v>1.92</v>
       </c>
     </row>
     <row r="228" spans="1:2">
@@ -3798,7 +3798,7 @@
         <v>228</v>
       </c>
       <c r="B228">
-        <v>491.04</v>
+        <v>636.048</v>
       </c>
     </row>
     <row r="229" spans="1:2">
@@ -3806,7 +3806,7 @@
         <v>229</v>
       </c>
       <c r="B229">
-        <v>80.49999999999999</v>
+        <v>96.59999999999999</v>
       </c>
     </row>
     <row r="230" spans="1:2">
@@ -3814,7 +3814,7 @@
         <v>230</v>
       </c>
       <c r="B230">
-        <v>492.48</v>
+        <v>590.976</v>
       </c>
     </row>
     <row r="231" spans="1:2">
@@ -3822,7 +3822,7 @@
         <v>231</v>
       </c>
       <c r="B231">
-        <v>195.96</v>
+        <v>235.152</v>
       </c>
     </row>
     <row r="232" spans="1:2">
@@ -3830,7 +3830,7 @@
         <v>232</v>
       </c>
       <c r="B232">
-        <v>9</v>
+        <v>10.8</v>
       </c>
     </row>
     <row r="233" spans="1:2">
@@ -3838,7 +3838,7 @@
         <v>233</v>
       </c>
       <c r="B233">
-        <v>1.44</v>
+        <v>1.728</v>
       </c>
     </row>
     <row r="234" spans="1:2">
@@ -3846,7 +3846,7 @@
         <v>234</v>
       </c>
       <c r="B234">
-        <v>417.9999999999999</v>
+        <v>501.6</v>
       </c>
     </row>
     <row r="235" spans="1:2">
@@ -3854,7 +3854,7 @@
         <v>235</v>
       </c>
       <c r="B235">
-        <v>323.84</v>
+        <v>388.608</v>
       </c>
     </row>
     <row r="236" spans="1:2">
@@ -3862,7 +3862,7 @@
         <v>236</v>
       </c>
       <c r="B236">
-        <v>346.3800000000001</v>
+        <v>415.656</v>
       </c>
     </row>
     <row r="237" spans="1:2">
@@ -3870,7 +3870,7 @@
         <v>237</v>
       </c>
       <c r="B237">
-        <v>514.96</v>
+        <v>617.9519999999999</v>
       </c>
     </row>
     <row r="238" spans="1:2">
@@ -3878,7 +3878,7 @@
         <v>238</v>
       </c>
       <c r="B238">
-        <v>12.8</v>
+        <v>15.36</v>
       </c>
     </row>
     <row r="239" spans="1:2">
@@ -3886,7 +3886,7 @@
         <v>239</v>
       </c>
       <c r="B239">
-        <v>395.3</v>
+        <v>474.36</v>
       </c>
     </row>
     <row r="240" spans="1:2">
@@ -3894,7 +3894,7 @@
         <v>240</v>
       </c>
       <c r="B240">
-        <v>386.4</v>
+        <v>463.6800000000001</v>
       </c>
     </row>
     <row r="241" spans="1:2">
@@ -3902,7 +3902,7 @@
         <v>241</v>
       </c>
       <c r="B241">
-        <v>107.46</v>
+        <v>128.952</v>
       </c>
     </row>
     <row r="242" spans="1:2">
@@ -3910,7 +3910,7 @@
         <v>242</v>
       </c>
       <c r="B242">
-        <v>204.6</v>
+        <v>245.52</v>
       </c>
     </row>
     <row r="243" spans="1:2">
@@ -3918,7 +3918,7 @@
         <v>243</v>
       </c>
       <c r="B243">
-        <v>310</v>
+        <v>372</v>
       </c>
     </row>
     <row r="244" spans="1:2">
@@ -3926,7 +3926,7 @@
         <v>244</v>
       </c>
       <c r="B244">
-        <v>6.999999999999999</v>
+        <v>8.4</v>
       </c>
     </row>
     <row r="245" spans="1:2">
@@ -3934,7 +3934,7 @@
         <v>245</v>
       </c>
       <c r="B245">
-        <v>15.9</v>
+        <v>19.08</v>
       </c>
     </row>
     <row r="246" spans="1:2">
@@ -3942,7 +3942,7 @@
         <v>246</v>
       </c>
       <c r="B246">
-        <v>397.16</v>
+        <v>481.392</v>
       </c>
     </row>
     <row r="247" spans="1:2">
@@ -3950,7 +3950,7 @@
         <v>247</v>
       </c>
       <c r="B247">
-        <v>300.56</v>
+        <v>360.672</v>
       </c>
     </row>
     <row r="248" spans="1:2">
@@ -3958,7 +3958,7 @@
         <v>248</v>
       </c>
       <c r="B248">
-        <v>240.3</v>
+        <v>288.36</v>
       </c>
     </row>
     <row r="249" spans="1:2">
@@ -3966,7 +3966,7 @@
         <v>249</v>
       </c>
       <c r="B249">
-        <v>629.16</v>
+        <v>816.1919999999999</v>
       </c>
     </row>
     <row r="250" spans="1:2">
@@ -3974,7 +3974,7 @@
         <v>250</v>
       </c>
       <c r="B250">
-        <v>137.52</v>
+        <v>165.024</v>
       </c>
     </row>
     <row r="251" spans="1:2">
@@ -3982,7 +3982,7 @@
         <v>251</v>
       </c>
       <c r="B251">
-        <v>96.48</v>
+        <v>115.776</v>
       </c>
     </row>
     <row r="252" spans="1:2">
@@ -3990,7 +3990,7 @@
         <v>252</v>
       </c>
       <c r="B252">
-        <v>32.8</v>
+        <v>39.36</v>
       </c>
     </row>
     <row r="253" spans="1:2">
@@ -3998,7 +3998,7 @@
         <v>253</v>
       </c>
       <c r="B253">
-        <v>40.88</v>
+        <v>49.056</v>
       </c>
     </row>
     <row r="254" spans="1:2">
@@ -4006,7 +4006,7 @@
         <v>254</v>
       </c>
       <c r="B254">
-        <v>226.44</v>
+        <v>271.728</v>
       </c>
     </row>
     <row r="255" spans="1:2">
@@ -4014,7 +4014,7 @@
         <v>255</v>
       </c>
       <c r="B255">
-        <v>233.84</v>
+        <v>280.608</v>
       </c>
     </row>
     <row r="256" spans="1:2">
@@ -4022,7 +4022,7 @@
         <v>256</v>
       </c>
       <c r="B256">
-        <v>19.44</v>
+        <v>23.328</v>
       </c>
     </row>
     <row r="257" spans="1:2">
@@ -4030,7 +4030,7 @@
         <v>257</v>
       </c>
       <c r="B257">
-        <v>32.24</v>
+        <v>38.688</v>
       </c>
     </row>
     <row r="258" spans="1:2">
@@ -4038,7 +4038,7 @@
         <v>258</v>
       </c>
       <c r="B258">
-        <v>388.36</v>
+        <v>466.032</v>
       </c>
     </row>
     <row r="259" spans="1:2">
@@ -4046,7 +4046,7 @@
         <v>259</v>
       </c>
       <c r="B259">
-        <v>240.9</v>
+        <v>289.08</v>
       </c>
     </row>
     <row r="260" spans="1:2">
@@ -4054,7 +4054,7 @@
         <v>260</v>
       </c>
       <c r="B260">
-        <v>15.04</v>
+        <v>18.048</v>
       </c>
     </row>
     <row r="261" spans="1:2">
@@ -4062,7 +4062,7 @@
         <v>261</v>
       </c>
       <c r="B261">
-        <v>378.1199999999999</v>
+        <v>453.744</v>
       </c>
     </row>
     <row r="262" spans="1:2">
@@ -4070,7 +4070,7 @@
         <v>262</v>
       </c>
       <c r="B262">
-        <v>410.4</v>
+        <v>492.48</v>
       </c>
     </row>
     <row r="263" spans="1:2">
@@ -4078,7 +4078,7 @@
         <v>263</v>
       </c>
       <c r="B263">
-        <v>297.48</v>
+        <v>356.976</v>
       </c>
     </row>
     <row r="264" spans="1:2">
@@ -4086,7 +4086,7 @@
         <v>264</v>
       </c>
       <c r="B264">
-        <v>489.0000000000001</v>
+        <v>586.8</v>
       </c>
     </row>
     <row r="265" spans="1:2">
@@ -4094,7 +4094,7 @@
         <v>265</v>
       </c>
       <c r="B265">
-        <v>17.7</v>
+        <v>21.24</v>
       </c>
     </row>
     <row r="266" spans="1:2">
@@ -4102,7 +4102,7 @@
         <v>266</v>
       </c>
       <c r="B266">
-        <v>49.20000000000001</v>
+        <v>59.04</v>
       </c>
     </row>
     <row r="267" spans="1:2">
@@ -4110,7 +4110,7 @@
         <v>267</v>
       </c>
       <c r="B267">
-        <v>36.16</v>
+        <v>43.392</v>
       </c>
     </row>
     <row r="268" spans="1:2">
@@ -4118,7 +4118,7 @@
         <v>268</v>
       </c>
       <c r="B268">
-        <v>293.5599999999999</v>
+        <v>352.272</v>
       </c>
     </row>
     <row r="269" spans="1:2">
@@ -4126,7 +4126,7 @@
         <v>269</v>
       </c>
       <c r="B269">
-        <v>485.1</v>
+        <v>582.12</v>
       </c>
     </row>
     <row r="270" spans="1:2">
@@ -4134,7 +4134,7 @@
         <v>270</v>
       </c>
       <c r="B270">
-        <v>442.8</v>
+        <v>531.36</v>
       </c>
     </row>
     <row r="271" spans="1:2">
@@ -4142,7 +4142,7 @@
         <v>271</v>
       </c>
       <c r="B271">
-        <v>366.56</v>
+        <v>439.872</v>
       </c>
     </row>
     <row r="272" spans="1:2">
@@ -4150,7 +4150,7 @@
         <v>272</v>
       </c>
       <c r="B272">
-        <v>366.36</v>
+        <v>439.6319999999999</v>
       </c>
     </row>
     <row r="273" spans="1:2">
@@ -4158,7 +4158,7 @@
         <v>273</v>
       </c>
       <c r="B273">
-        <v>292</v>
+        <v>350.4</v>
       </c>
     </row>
     <row r="274" spans="1:2">
@@ -4166,7 +4166,7 @@
         <v>274</v>
       </c>
       <c r="B274">
-        <v>370</v>
+        <v>444</v>
       </c>
     </row>
     <row r="275" spans="1:2">
@@ -4174,7 +4174,7 @@
         <v>275</v>
       </c>
       <c r="B275">
-        <v>127.92</v>
+        <v>153.504</v>
       </c>
     </row>
     <row r="276" spans="1:2">
@@ -4182,7 +4182,7 @@
         <v>276</v>
       </c>
       <c r="B276">
-        <v>241.92</v>
+        <v>290.304</v>
       </c>
     </row>
     <row r="277" spans="1:2">
@@ -4190,7 +4190,7 @@
         <v>277</v>
       </c>
       <c r="B277">
-        <v>15.96</v>
+        <v>19.152</v>
       </c>
     </row>
     <row r="278" spans="1:2">
@@ -4198,7 +4198,7 @@
         <v>278</v>
       </c>
       <c r="B278">
-        <v>65.2</v>
+        <v>78.23999999999999</v>
       </c>
     </row>
     <row r="279" spans="1:2">
@@ -4206,7 +4206,7 @@
         <v>279</v>
       </c>
       <c r="B279">
-        <v>315.36</v>
+        <v>378.432</v>
       </c>
     </row>
     <row r="280" spans="1:2">
@@ -4214,7 +4214,7 @@
         <v>280</v>
       </c>
       <c r="B280">
-        <v>278.3200000000001</v>
+        <v>333.984</v>
       </c>
     </row>
     <row r="281" spans="1:2">
@@ -4222,7 +4222,7 @@
         <v>281</v>
       </c>
       <c r="B281">
-        <v>486.48</v>
+        <v>588.576</v>
       </c>
     </row>
     <row r="282" spans="1:2">
@@ -4230,7 +4230,7 @@
         <v>282</v>
       </c>
       <c r="B282">
-        <v>0.4</v>
+        <v>0.48</v>
       </c>
     </row>
     <row r="283" spans="1:2">
@@ -4238,7 +4238,7 @@
         <v>283</v>
       </c>
       <c r="B283">
-        <v>248.4</v>
+        <v>298.08</v>
       </c>
     </row>
     <row r="284" spans="1:2">
@@ -4246,7 +4246,7 @@
         <v>284</v>
       </c>
       <c r="B284">
-        <v>393.6000000000001</v>
+        <v>472.32</v>
       </c>
     </row>
     <row r="285" spans="1:2">
@@ -4254,7 +4254,7 @@
         <v>285</v>
       </c>
       <c r="B285">
-        <v>155.52</v>
+        <v>186.624</v>
       </c>
     </row>
     <row r="286" spans="1:2">
@@ -4262,7 +4262,7 @@
         <v>286</v>
       </c>
       <c r="B286">
-        <v>106.7</v>
+        <v>128.04</v>
       </c>
     </row>
     <row r="287" spans="1:2">
@@ -4270,7 +4270,7 @@
         <v>287</v>
       </c>
       <c r="B287">
-        <v>131.04</v>
+        <v>157.248</v>
       </c>
     </row>
     <row r="288" spans="1:2">
@@ -4278,7 +4278,7 @@
         <v>288</v>
       </c>
       <c r="B288">
-        <v>32.2</v>
+        <v>38.64</v>
       </c>
     </row>
     <row r="289" spans="1:2">
@@ -4286,7 +4286,7 @@
         <v>289</v>
       </c>
       <c r="B289">
-        <v>92.22</v>
+        <v>110.664</v>
       </c>
     </row>
     <row r="290" spans="1:2">
@@ -4294,7 +4294,7 @@
         <v>290</v>
       </c>
       <c r="B290">
-        <v>462.0799999999999</v>
+        <v>554.496</v>
       </c>
     </row>
     <row r="291" spans="1:2">
@@ -4302,7 +4302,7 @@
         <v>291</v>
       </c>
       <c r="B291">
-        <v>80.7</v>
+        <v>96.84</v>
       </c>
     </row>
     <row r="292" spans="1:2">
@@ -4310,7 +4310,7 @@
         <v>292</v>
       </c>
       <c r="B292">
-        <v>7.000000000000001</v>
+        <v>8.4</v>
       </c>
     </row>
     <row r="293" spans="1:2">
@@ -4318,7 +4318,7 @@
         <v>293</v>
       </c>
       <c r="B293">
-        <v>278.76</v>
+        <v>334.512</v>
       </c>
     </row>
     <row r="294" spans="1:2">
@@ -4326,7 +4326,7 @@
         <v>294</v>
       </c>
       <c r="B294">
-        <v>41.94</v>
+        <v>50.328</v>
       </c>
     </row>
     <row r="295" spans="1:2">
@@ -4334,7 +4334,7 @@
         <v>295</v>
       </c>
       <c r="B295">
-        <v>50.82</v>
+        <v>60.98399999999999</v>
       </c>
     </row>
     <row r="296" spans="1:2">
@@ -4342,7 +4342,7 @@
         <v>296</v>
       </c>
       <c r="B296">
-        <v>27.2</v>
+        <v>32.64</v>
       </c>
     </row>
     <row r="297" spans="1:2">
@@ -4350,7 +4350,7 @@
         <v>297</v>
       </c>
       <c r="B297">
-        <v>373.46</v>
+        <v>448.152</v>
       </c>
     </row>
     <row r="298" spans="1:2">
@@ -4358,7 +4358,7 @@
         <v>298</v>
       </c>
       <c r="B298">
-        <v>145</v>
+        <v>174</v>
       </c>
     </row>
     <row r="299" spans="1:2">
@@ -4366,7 +4366,7 @@
         <v>299</v>
       </c>
       <c r="B299">
-        <v>558.36</v>
+        <v>731.232</v>
       </c>
     </row>
     <row r="300" spans="1:2">
@@ -4374,7 +4374,7 @@
         <v>300</v>
       </c>
       <c r="B300">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="301" spans="1:2">
@@ -4382,7 +4382,7 @@
         <v>301</v>
       </c>
       <c r="B301">
-        <v>225.78</v>
+        <v>270.936</v>
       </c>
     </row>
     <row r="302" spans="1:2">
@@ -4390,7 +4390,7 @@
         <v>302</v>
       </c>
       <c r="B302">
-        <v>182.16</v>
+        <v>218.592</v>
       </c>
     </row>
     <row r="303" spans="1:2">
@@ -4398,7 +4398,7 @@
         <v>303</v>
       </c>
       <c r="B303">
-        <v>346.32</v>
+        <v>415.5839999999999</v>
       </c>
     </row>
     <row r="304" spans="1:2">
@@ -4406,7 +4406,7 @@
         <v>304</v>
       </c>
       <c r="B304">
-        <v>337.92</v>
+        <v>405.504</v>
       </c>
     </row>
     <row r="305" spans="1:2">
@@ -4414,7 +4414,7 @@
         <v>305</v>
       </c>
       <c r="B305">
-        <v>330.4</v>
+        <v>396.48</v>
       </c>
     </row>
     <row r="306" spans="1:2">
@@ -4422,7 +4422,7 @@
         <v>306</v>
       </c>
       <c r="B306">
-        <v>502.3200000000001</v>
+        <v>602.7840000000001</v>
       </c>
     </row>
     <row r="307" spans="1:2">
@@ -4430,7 +4430,7 @@
         <v>307</v>
       </c>
       <c r="B307">
-        <v>161.2</v>
+        <v>193.44</v>
       </c>
     </row>
     <row r="308" spans="1:2">
@@ -4438,7 +4438,7 @@
         <v>308</v>
       </c>
       <c r="B308">
-        <v>0.4</v>
+        <v>0.48</v>
       </c>
     </row>
     <row r="309" spans="1:2">
@@ -4446,7 +4446,7 @@
         <v>309</v>
       </c>
       <c r="B309">
-        <v>278.86</v>
+        <v>334.632</v>
       </c>
     </row>
     <row r="310" spans="1:2">
@@ -4454,7 +4454,7 @@
         <v>310</v>
       </c>
       <c r="B310">
-        <v>273.24</v>
+        <v>327.888</v>
       </c>
     </row>
     <row r="311" spans="1:2">
@@ -4462,7 +4462,7 @@
         <v>311</v>
       </c>
       <c r="B311">
-        <v>43.2</v>
+        <v>51.84</v>
       </c>
     </row>
     <row r="312" spans="1:2">
@@ -4470,7 +4470,7 @@
         <v>312</v>
       </c>
       <c r="B312">
-        <v>229.46</v>
+        <v>275.352</v>
       </c>
     </row>
     <row r="313" spans="1:2">
@@ -4478,7 +4478,7 @@
         <v>313</v>
       </c>
       <c r="B313">
-        <v>247.16</v>
+        <v>296.592</v>
       </c>
     </row>
     <row r="314" spans="1:2">
@@ -4486,7 +4486,7 @@
         <v>314</v>
       </c>
       <c r="B314">
-        <v>67.08</v>
+        <v>80.496</v>
       </c>
     </row>
     <row r="315" spans="1:2">
@@ -4494,7 +4494,7 @@
         <v>315</v>
       </c>
       <c r="B315">
-        <v>409.92</v>
+        <v>496.704</v>
       </c>
     </row>
     <row r="316" spans="1:2">
@@ -4502,7 +4502,7 @@
         <v>316</v>
       </c>
       <c r="B316">
-        <v>332.8800000000001</v>
+        <v>399.456</v>
       </c>
     </row>
     <row r="317" spans="1:2">
@@ -4510,7 +4510,7 @@
         <v>317</v>
       </c>
       <c r="B317">
-        <v>196.56</v>
+        <v>235.872</v>
       </c>
     </row>
     <row r="318" spans="1:2">
@@ -4518,7 +4518,7 @@
         <v>318</v>
       </c>
       <c r="B318">
-        <v>4</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="319" spans="1:2">
@@ -4526,7 +4526,7 @@
         <v>319</v>
       </c>
       <c r="B319">
-        <v>425.8799999999999</v>
+        <v>511.0559999999999</v>
       </c>
     </row>
     <row r="320" spans="1:2">
@@ -4534,7 +4534,7 @@
         <v>320</v>
       </c>
       <c r="B320">
-        <v>312.32</v>
+        <v>374.784</v>
       </c>
     </row>
     <row r="321" spans="1:2">
@@ -4542,7 +4542,7 @@
         <v>321</v>
       </c>
       <c r="B321">
-        <v>3.6</v>
+        <v>4.32</v>
       </c>
     </row>
     <row r="322" spans="1:2">
@@ -4550,7 +4550,7 @@
         <v>322</v>
       </c>
       <c r="B322">
-        <v>192.66</v>
+        <v>231.192</v>
       </c>
     </row>
     <row r="323" spans="1:2">
@@ -4558,7 +4558,7 @@
         <v>323</v>
       </c>
       <c r="B323">
-        <v>584.8199999999999</v>
+        <v>701.784</v>
       </c>
     </row>
     <row r="324" spans="1:2">
@@ -4566,7 +4566,7 @@
         <v>324</v>
       </c>
       <c r="B324">
-        <v>340.48</v>
+        <v>408.576</v>
       </c>
     </row>
     <row r="325" spans="1:2">
@@ -4574,7 +4574,7 @@
         <v>325</v>
       </c>
       <c r="B325">
-        <v>1.6</v>
+        <v>1.92</v>
       </c>
     </row>
     <row r="326" spans="1:2">
@@ -4582,7 +4582,7 @@
         <v>326</v>
       </c>
       <c r="B326">
-        <v>17.86</v>
+        <v>21.432</v>
       </c>
     </row>
     <row r="327" spans="1:2">
@@ -4590,7 +4590,7 @@
         <v>327</v>
       </c>
       <c r="B327">
-        <v>353.16</v>
+        <v>423.792</v>
       </c>
     </row>
     <row r="328" spans="1:2">
@@ -4598,7 +4598,7 @@
         <v>328</v>
       </c>
       <c r="B328">
-        <v>123.5</v>
+        <v>148.2</v>
       </c>
     </row>
     <row r="329" spans="1:2">
@@ -4606,7 +4606,7 @@
         <v>329</v>
       </c>
       <c r="B329">
-        <v>59.76000000000001</v>
+        <v>71.712</v>
       </c>
     </row>
     <row r="330" spans="1:2">
@@ -4614,7 +4614,7 @@
         <v>330</v>
       </c>
       <c r="B330">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="331" spans="1:2">
@@ -4622,7 +4622,7 @@
         <v>331</v>
       </c>
       <c r="B331">
-        <v>10.64</v>
+        <v>12.768</v>
       </c>
     </row>
     <row r="332" spans="1:2">
@@ -4630,7 +4630,7 @@
         <v>332</v>
       </c>
       <c r="B332">
-        <v>218.4</v>
+        <v>262.08</v>
       </c>
     </row>
     <row r="333" spans="1:2">
@@ -4638,7 +4638,7 @@
         <v>333</v>
       </c>
       <c r="B333">
-        <v>1.2</v>
+        <v>1.44</v>
       </c>
     </row>
     <row r="334" spans="1:2">
@@ -4646,7 +4646,7 @@
         <v>334</v>
       </c>
       <c r="B334">
-        <v>223.3</v>
+        <v>267.96</v>
       </c>
     </row>
     <row r="335" spans="1:2">
@@ -4654,7 +4654,7 @@
         <v>335</v>
       </c>
       <c r="B335">
-        <v>146.4</v>
+        <v>175.68</v>
       </c>
     </row>
     <row r="336" spans="1:2">
@@ -4662,7 +4662,7 @@
         <v>336</v>
       </c>
       <c r="B336">
-        <v>56.58000000000001</v>
+        <v>67.896</v>
       </c>
     </row>
     <row r="337" spans="1:2">
@@ -4670,7 +4670,7 @@
         <v>337</v>
       </c>
       <c r="B337">
-        <v>596.9599999999999</v>
+        <v>716.3519999999999</v>
       </c>
     </row>
     <row r="338" spans="1:2">
@@ -4678,7 +4678,7 @@
         <v>338</v>
       </c>
       <c r="B338">
-        <v>267.4</v>
+        <v>320.88</v>
       </c>
     </row>
     <row r="339" spans="1:2">
@@ -4686,7 +4686,7 @@
         <v>339</v>
       </c>
       <c r="B339">
-        <v>388.6799999999999</v>
+        <v>466.4159999999999</v>
       </c>
     </row>
     <row r="340" spans="1:2">
@@ -4694,7 +4694,7 @@
         <v>340</v>
       </c>
       <c r="B340">
-        <v>25.2</v>
+        <v>30.24</v>
       </c>
     </row>
     <row r="341" spans="1:2">
@@ -4702,7 +4702,7 @@
         <v>341</v>
       </c>
       <c r="B341">
-        <v>421.48</v>
+        <v>505.776</v>
       </c>
     </row>
     <row r="342" spans="1:2">
@@ -4710,7 +4710,7 @@
         <v>342</v>
       </c>
       <c r="B342">
-        <v>228.76</v>
+        <v>274.512</v>
       </c>
     </row>
     <row r="343" spans="1:2">
@@ -4718,7 +4718,7 @@
         <v>343</v>
       </c>
       <c r="B343">
-        <v>299.2</v>
+        <v>359.04</v>
       </c>
     </row>
     <row r="344" spans="1:2">
@@ -4726,7 +4726,7 @@
         <v>344</v>
       </c>
       <c r="B344">
-        <v>533.72</v>
+        <v>645.264</v>
       </c>
     </row>
     <row r="345" spans="1:2">
@@ -4734,7 +4734,7 @@
         <v>345</v>
       </c>
       <c r="B345">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="346" spans="1:2">
@@ -4742,7 +4742,7 @@
         <v>346</v>
       </c>
       <c r="B346">
-        <v>171.36</v>
+        <v>205.632</v>
       </c>
     </row>
     <row r="347" spans="1:2">
@@ -4750,7 +4750,7 @@
         <v>347</v>
       </c>
       <c r="B347">
-        <v>208.08</v>
+        <v>249.696</v>
       </c>
     </row>
     <row r="348" spans="1:2">
@@ -4758,7 +4758,7 @@
         <v>348</v>
       </c>
       <c r="B348">
-        <v>1.6</v>
+        <v>1.92</v>
       </c>
     </row>
     <row r="349" spans="1:2">
@@ -4766,7 +4766,7 @@
         <v>349</v>
       </c>
       <c r="B349">
-        <v>1.8</v>
+        <v>2.16</v>
       </c>
     </row>
     <row r="350" spans="1:2">
@@ -4774,7 +4774,7 @@
         <v>350</v>
       </c>
       <c r="B350">
-        <v>516.6</v>
+        <v>619.92</v>
       </c>
     </row>
     <row r="351" spans="1:2">
@@ -4782,7 +4782,7 @@
         <v>351</v>
       </c>
       <c r="B351">
-        <v>160.8</v>
+        <v>192.96</v>
       </c>
     </row>
     <row r="352" spans="1:2">
@@ -4790,7 +4790,7 @@
         <v>352</v>
       </c>
       <c r="B352">
-        <v>19.56</v>
+        <v>23.472</v>
       </c>
     </row>
     <row r="353" spans="1:2">
@@ -4798,7 +4798,7 @@
         <v>353</v>
       </c>
       <c r="B353">
-        <v>289.44</v>
+        <v>347.328</v>
       </c>
     </row>
     <row r="354" spans="1:2">
@@ -4806,7 +4806,7 @@
         <v>354</v>
       </c>
       <c r="B354">
-        <v>394.2</v>
+        <v>473.04</v>
       </c>
     </row>
     <row r="355" spans="1:2">
@@ -4814,7 +4814,7 @@
         <v>355</v>
       </c>
       <c r="B355">
-        <v>4.98</v>
+        <v>5.976</v>
       </c>
     </row>
     <row r="356" spans="1:2">
@@ -4822,7 +4822,7 @@
         <v>356</v>
       </c>
       <c r="B356">
-        <v>35.2</v>
+        <v>42.23999999999999</v>
       </c>
     </row>
     <row r="357" spans="1:2">
@@ -4830,7 +4830,7 @@
         <v>357</v>
       </c>
       <c r="B357">
-        <v>71.92</v>
+        <v>86.30399999999999</v>
       </c>
     </row>
     <row r="358" spans="1:2">
@@ -4838,7 +4838,7 @@
         <v>358</v>
       </c>
       <c r="B358">
-        <v>249.6</v>
+        <v>299.52</v>
       </c>
     </row>
     <row r="359" spans="1:2">
@@ -4846,7 +4846,7 @@
         <v>359</v>
       </c>
       <c r="B359">
-        <v>83.41999999999999</v>
+        <v>100.104</v>
       </c>
     </row>
     <row r="360" spans="1:2">
@@ -4854,7 +4854,7 @@
         <v>360</v>
       </c>
       <c r="B360">
-        <v>4.2</v>
+        <v>5.04</v>
       </c>
     </row>
     <row r="361" spans="1:2">
@@ -4862,7 +4862,7 @@
         <v>361</v>
       </c>
       <c r="B361">
-        <v>384.3</v>
+        <v>507.96</v>
       </c>
     </row>
     <row r="362" spans="1:2">
@@ -4870,7 +4870,7 @@
         <v>362</v>
       </c>
       <c r="B362">
-        <v>513.54</v>
+        <v>616.2479999999999</v>
       </c>
     </row>
     <row r="363" spans="1:2">
@@ -4878,7 +4878,7 @@
         <v>363</v>
       </c>
       <c r="B363">
-        <v>212</v>
+        <v>254.4</v>
       </c>
     </row>
     <row r="364" spans="1:2">
@@ -4886,7 +4886,7 @@
         <v>364</v>
       </c>
       <c r="B364">
-        <v>104.64</v>
+        <v>125.568</v>
       </c>
     </row>
     <row r="365" spans="1:2">
@@ -4894,7 +4894,7 @@
         <v>365</v>
       </c>
       <c r="B365">
-        <v>283.8</v>
+        <v>340.56</v>
       </c>
     </row>
     <row r="366" spans="1:2">
@@ -4902,7 +4902,7 @@
         <v>366</v>
       </c>
       <c r="B366">
-        <v>306.36</v>
+        <v>367.6319999999999</v>
       </c>
     </row>
     <row r="367" spans="1:2">
@@ -4910,7 +4910,7 @@
         <v>367</v>
       </c>
       <c r="B367">
-        <v>203</v>
+        <v>243.6</v>
       </c>
     </row>
     <row r="368" spans="1:2">
@@ -4918,7 +4918,7 @@
         <v>368</v>
       </c>
       <c r="B368">
-        <v>99.22</v>
+        <v>119.064</v>
       </c>
     </row>
     <row r="369" spans="1:2">
@@ -4926,7 +4926,7 @@
         <v>369</v>
       </c>
       <c r="B369">
-        <v>6.48</v>
+        <v>7.776</v>
       </c>
     </row>
     <row r="370" spans="1:2">
@@ -4934,7 +4934,7 @@
         <v>370</v>
       </c>
       <c r="B370">
-        <v>7.98</v>
+        <v>9.575999999999999</v>
       </c>
     </row>
     <row r="371" spans="1:2">
@@ -4942,7 +4942,7 @@
         <v>371</v>
       </c>
       <c r="B371">
-        <v>94.2</v>
+        <v>113.04</v>
       </c>
     </row>
     <row r="372" spans="1:2">
@@ -4950,7 +4950,7 @@
         <v>372</v>
       </c>
       <c r="B372">
-        <v>83.3</v>
+        <v>99.95999999999999</v>
       </c>
     </row>
     <row r="373" spans="1:2">
@@ -4958,7 +4958,7 @@
         <v>373</v>
       </c>
       <c r="B373">
-        <v>380.3799999999999</v>
+        <v>456.456</v>
       </c>
     </row>
     <row r="374" spans="1:2">
@@ -4966,7 +4966,7 @@
         <v>374</v>
       </c>
       <c r="B374">
-        <v>341.64</v>
+        <v>409.968</v>
       </c>
     </row>
     <row r="375" spans="1:2">
@@ -4974,7 +4974,7 @@
         <v>375</v>
       </c>
       <c r="B375">
-        <v>417.1199999999999</v>
+        <v>500.544</v>
       </c>
     </row>
     <row r="376" spans="1:2">
@@ -4982,7 +4982,7 @@
         <v>376</v>
       </c>
       <c r="B376">
-        <v>328.9999999999999</v>
+        <v>394.8</v>
       </c>
     </row>
     <row r="377" spans="1:2">
@@ -4990,7 +4990,7 @@
         <v>377</v>
       </c>
       <c r="B377">
-        <v>75.60000000000001</v>
+        <v>90.72</v>
       </c>
     </row>
     <row r="378" spans="1:2">
@@ -4998,7 +4998,7 @@
         <v>378</v>
       </c>
       <c r="B378">
-        <v>230.46</v>
+        <v>276.552</v>
       </c>
     </row>
     <row r="379" spans="1:2">
@@ -5006,7 +5006,7 @@
         <v>379</v>
       </c>
       <c r="B379">
-        <v>277.2</v>
+        <v>332.64</v>
       </c>
     </row>
     <row r="380" spans="1:2">
@@ -5014,7 +5014,7 @@
         <v>380</v>
       </c>
       <c r="B380">
-        <v>230.68</v>
+        <v>276.816</v>
       </c>
     </row>
     <row r="381" spans="1:2">
@@ -5022,7 +5022,7 @@
         <v>381</v>
       </c>
       <c r="B381">
-        <v>70.72</v>
+        <v>84.86399999999999</v>
       </c>
     </row>
     <row r="382" spans="1:2">
@@ -5030,7 +5030,7 @@
         <v>382</v>
       </c>
       <c r="B382">
-        <v>70.56</v>
+        <v>84.672</v>
       </c>
     </row>
     <row r="383" spans="1:2">
@@ -5038,7 +5038,7 @@
         <v>383</v>
       </c>
       <c r="B383">
-        <v>930</v>
+        <v>1242</v>
       </c>
     </row>
     <row r="384" spans="1:2">
@@ -5046,7 +5046,7 @@
         <v>384</v>
       </c>
       <c r="B384">
-        <v>355.6799999999999</v>
+        <v>426.816</v>
       </c>
     </row>
     <row r="385" spans="1:2">
@@ -5054,7 +5054,7 @@
         <v>385</v>
       </c>
       <c r="B385">
-        <v>4.399999999999999</v>
+        <v>5.279999999999999</v>
       </c>
     </row>
     <row r="386" spans="1:2">
@@ -5062,7 +5062,7 @@
         <v>386</v>
       </c>
       <c r="B386">
-        <v>134.2</v>
+        <v>161.04</v>
       </c>
     </row>
     <row r="387" spans="1:2">
@@ -5070,7 +5070,7 @@
         <v>387</v>
       </c>
       <c r="B387">
-        <v>445.4999999999999</v>
+        <v>534.6</v>
       </c>
     </row>
     <row r="388" spans="1:2">
@@ -5078,7 +5078,7 @@
         <v>388</v>
       </c>
       <c r="B388">
-        <v>194.58</v>
+        <v>233.496</v>
       </c>
     </row>
     <row r="389" spans="1:2">
@@ -5086,7 +5086,7 @@
         <v>389</v>
       </c>
       <c r="B389">
-        <v>5.6</v>
+        <v>6.72</v>
       </c>
     </row>
     <row r="390" spans="1:2">
@@ -5094,7 +5094,7 @@
         <v>390</v>
       </c>
       <c r="B390">
-        <v>24.48</v>
+        <v>29.376</v>
       </c>
     </row>
     <row r="391" spans="1:2">
@@ -5102,7 +5102,7 @@
         <v>391</v>
       </c>
       <c r="B391">
-        <v>148.8</v>
+        <v>178.56</v>
       </c>
     </row>
     <row r="392" spans="1:2">
@@ -5110,7 +5110,7 @@
         <v>392</v>
       </c>
       <c r="B392">
-        <v>214.5</v>
+        <v>257.4</v>
       </c>
     </row>
     <row r="393" spans="1:2">
@@ -5118,7 +5118,7 @@
         <v>393</v>
       </c>
       <c r="B393">
-        <v>138.24</v>
+        <v>165.888</v>
       </c>
     </row>
     <row r="394" spans="1:2">
@@ -5126,7 +5126,7 @@
         <v>394</v>
       </c>
       <c r="B394">
-        <v>254.2</v>
+        <v>305.04</v>
       </c>
     </row>
     <row r="395" spans="1:2">
@@ -5134,7 +5134,7 @@
         <v>395</v>
       </c>
       <c r="B395">
-        <v>0.7999999999999999</v>
+        <v>0.96</v>
       </c>
     </row>
     <row r="396" spans="1:2">
@@ -5142,7 +5142,7 @@
         <v>396</v>
       </c>
       <c r="B396">
-        <v>115.2</v>
+        <v>138.24</v>
       </c>
     </row>
     <row r="397" spans="1:2">
@@ -5150,7 +5150,7 @@
         <v>397</v>
       </c>
       <c r="B397">
-        <v>368.88</v>
+        <v>442.656</v>
       </c>
     </row>
     <row r="398" spans="1:2">
@@ -5158,7 +5158,7 @@
         <v>398</v>
       </c>
       <c r="B398">
-        <v>8.6</v>
+        <v>10.32</v>
       </c>
     </row>
     <row r="399" spans="1:2">
@@ -5166,7 +5166,7 @@
         <v>399</v>
       </c>
       <c r="B399">
-        <v>116.5</v>
+        <v>139.8</v>
       </c>
     </row>
     <row r="400" spans="1:2">
@@ -5174,7 +5174,7 @@
         <v>400</v>
       </c>
       <c r="B400">
-        <v>361.6199999999999</v>
+        <v>433.944</v>
       </c>
     </row>
     <row r="401" spans="1:2">
@@ -5182,7 +5182,7 @@
         <v>401</v>
       </c>
       <c r="B401">
-        <v>44.16</v>
+        <v>52.992</v>
       </c>
     </row>
     <row r="402" spans="1:2">
@@ -5190,7 +5190,7 @@
         <v>402</v>
       </c>
       <c r="B402">
-        <v>3</v>
+        <v>3.6</v>
       </c>
     </row>
     <row r="403" spans="1:2">
@@ -5198,7 +5198,7 @@
         <v>403</v>
       </c>
       <c r="B403">
-        <v>13.16</v>
+        <v>15.792</v>
       </c>
     </row>
     <row r="404" spans="1:2">
@@ -5206,7 +5206,7 @@
         <v>404</v>
       </c>
       <c r="B404">
-        <v>45.2</v>
+        <v>54.23999999999999</v>
       </c>
     </row>
     <row r="405" spans="1:2">
@@ -5214,7 +5214,7 @@
         <v>405</v>
       </c>
       <c r="B405">
-        <v>10.4</v>
+        <v>12.48</v>
       </c>
     </row>
     <row r="406" spans="1:2">
@@ -5222,7 +5222,7 @@
         <v>406</v>
       </c>
       <c r="B406">
-        <v>287.1199999999999</v>
+        <v>344.544</v>
       </c>
     </row>
     <row r="407" spans="1:2">
@@ -5230,7 +5230,7 @@
         <v>407</v>
       </c>
       <c r="B407">
-        <v>183.7</v>
+        <v>220.44</v>
       </c>
     </row>
     <row r="408" spans="1:2">
@@ -5238,7 +5238,7 @@
         <v>408</v>
       </c>
       <c r="B408">
-        <v>305.04</v>
+        <v>366.048</v>
       </c>
     </row>
     <row r="409" spans="1:2">
@@ -5246,7 +5246,7 @@
         <v>409</v>
       </c>
       <c r="B409">
-        <v>39.1</v>
+        <v>46.92</v>
       </c>
     </row>
     <row r="410" spans="1:2">
@@ -5254,7 +5254,7 @@
         <v>410</v>
       </c>
       <c r="B410">
-        <v>486.6399999999999</v>
+        <v>583.9680000000001</v>
       </c>
     </row>
     <row r="411" spans="1:2">
@@ -5262,7 +5262,7 @@
         <v>411</v>
       </c>
       <c r="B411">
-        <v>328.5</v>
+        <v>394.2</v>
       </c>
     </row>
     <row r="412" spans="1:2">
@@ -5270,7 +5270,7 @@
         <v>412</v>
       </c>
       <c r="B412">
-        <v>311.04</v>
+        <v>373.2479999999999</v>
       </c>
     </row>
     <row r="413" spans="1:2">
@@ -5278,7 +5278,7 @@
         <v>413</v>
       </c>
       <c r="B413">
-        <v>334.9599999999999</v>
+        <v>401.952</v>
       </c>
     </row>
     <row r="414" spans="1:2">
@@ -5286,7 +5286,7 @@
         <v>414</v>
       </c>
       <c r="B414">
-        <v>212.8</v>
+        <v>255.36</v>
       </c>
     </row>
     <row r="415" spans="1:2">
@@ -5294,7 +5294,7 @@
         <v>415</v>
       </c>
       <c r="B415">
-        <v>21</v>
+        <v>25.2</v>
       </c>
     </row>
     <row r="416" spans="1:2">
@@ -5302,7 +5302,7 @@
         <v>416</v>
       </c>
       <c r="B416">
-        <v>1.2</v>
+        <v>1.44</v>
       </c>
     </row>
     <row r="417" spans="1:2">
@@ -5310,7 +5310,7 @@
         <v>417</v>
       </c>
       <c r="B417">
-        <v>57.92</v>
+        <v>69.504</v>
       </c>
     </row>
     <row r="418" spans="1:2">
@@ -5318,7 +5318,7 @@
         <v>418</v>
       </c>
       <c r="B418">
-        <v>24.84</v>
+        <v>29.808</v>
       </c>
     </row>
     <row r="419" spans="1:2">
@@ -5326,7 +5326,7 @@
         <v>419</v>
       </c>
       <c r="B419">
-        <v>2.58</v>
+        <v>3.096</v>
       </c>
     </row>
     <row r="420" spans="1:2">
@@ -5334,7 +5334,7 @@
         <v>420</v>
       </c>
       <c r="B420">
-        <v>102.96</v>
+        <v>123.552</v>
       </c>
     </row>
     <row r="421" spans="1:2">
@@ -5342,7 +5342,7 @@
         <v>421</v>
       </c>
       <c r="B421">
-        <v>437.88</v>
+        <v>525.456</v>
       </c>
     </row>
     <row r="422" spans="1:2">
@@ -5350,7 +5350,7 @@
         <v>422</v>
       </c>
       <c r="B422">
-        <v>302.08</v>
+        <v>362.496</v>
       </c>
     </row>
     <row r="423" spans="1:2">
@@ -5358,7 +5358,7 @@
         <v>423</v>
       </c>
       <c r="B423">
-        <v>23.6</v>
+        <v>28.32</v>
       </c>
     </row>
     <row r="424" spans="1:2">
@@ -5366,7 +5366,7 @@
         <v>424</v>
       </c>
       <c r="B424">
-        <v>422.8</v>
+        <v>507.36</v>
       </c>
     </row>
     <row r="425" spans="1:2">
@@ -5374,7 +5374,7 @@
         <v>425</v>
       </c>
       <c r="B425">
-        <v>48.3</v>
+        <v>57.96</v>
       </c>
     </row>
     <row r="426" spans="1:2">
@@ -5382,7 +5382,7 @@
         <v>426</v>
       </c>
       <c r="B426">
-        <v>85.68000000000001</v>
+        <v>102.816</v>
       </c>
     </row>
     <row r="427" spans="1:2">
@@ -5390,7 +5390,7 @@
         <v>427</v>
       </c>
       <c r="B427">
-        <v>537.84</v>
+        <v>645.408</v>
       </c>
     </row>
     <row r="428" spans="1:2">
@@ -5398,7 +5398,7 @@
         <v>428</v>
       </c>
       <c r="B428">
-        <v>65</v>
+        <v>78</v>
       </c>
     </row>
     <row r="429" spans="1:2">
@@ -5406,7 +5406,7 @@
         <v>429</v>
       </c>
       <c r="B429">
-        <v>411.14</v>
+        <v>493.3680000000001</v>
       </c>
     </row>
     <row r="430" spans="1:2">
@@ -5414,7 +5414,7 @@
         <v>430</v>
       </c>
       <c r="B430">
-        <v>207.48</v>
+        <v>248.976</v>
       </c>
     </row>
     <row r="431" spans="1:2">
@@ -5422,7 +5422,7 @@
         <v>431</v>
       </c>
       <c r="B431">
-        <v>2.6</v>
+        <v>3.12</v>
       </c>
     </row>
     <row r="432" spans="1:2">
@@ -5430,7 +5430,7 @@
         <v>432</v>
       </c>
       <c r="B432">
-        <v>67.61999999999999</v>
+        <v>81.14399999999999</v>
       </c>
     </row>
     <row r="433" spans="1:2">
@@ -5438,7 +5438,7 @@
         <v>433</v>
       </c>
       <c r="B433">
-        <v>340.6</v>
+        <v>408.72</v>
       </c>
     </row>
     <row r="434" spans="1:2">
@@ -5446,7 +5446,7 @@
         <v>434</v>
       </c>
       <c r="B434">
-        <v>84.00000000000001</v>
+        <v>100.8</v>
       </c>
     </row>
     <row r="435" spans="1:2">
@@ -5454,7 +5454,7 @@
         <v>435</v>
       </c>
       <c r="B435">
-        <v>120</v>
+        <v>144</v>
       </c>
     </row>
     <row r="436" spans="1:2">
@@ -5462,7 +5462,7 @@
         <v>436</v>
       </c>
       <c r="B436">
-        <v>414.4</v>
+        <v>497.28</v>
       </c>
     </row>
     <row r="437" spans="1:2">
@@ -5470,7 +5470,7 @@
         <v>437</v>
       </c>
       <c r="B437">
-        <v>451.22</v>
+        <v>541.4639999999999</v>
       </c>
     </row>
     <row r="438" spans="1:2">
@@ -5478,7 +5478,7 @@
         <v>438</v>
       </c>
       <c r="B438">
-        <v>246.72</v>
+        <v>296.064</v>
       </c>
     </row>
     <row r="439" spans="1:2">
@@ -5486,7 +5486,7 @@
         <v>439</v>
       </c>
       <c r="B439">
-        <v>362.6</v>
+        <v>435.12</v>
       </c>
     </row>
     <row r="440" spans="1:2">
@@ -5494,7 +5494,7 @@
         <v>440</v>
       </c>
       <c r="B440">
-        <v>68.64</v>
+        <v>82.36799999999999</v>
       </c>
     </row>
     <row r="441" spans="1:2">
@@ -5502,7 +5502,7 @@
         <v>441</v>
       </c>
       <c r="B441">
-        <v>461.76</v>
+        <v>554.112</v>
       </c>
     </row>
     <row r="442" spans="1:2">
@@ -5510,7 +5510,7 @@
         <v>442</v>
       </c>
       <c r="B442">
-        <v>328.5</v>
+        <v>394.2</v>
       </c>
     </row>
     <row r="443" spans="1:2">
@@ -5518,7 +5518,7 @@
         <v>443</v>
       </c>
       <c r="B443">
-        <v>415.4</v>
+        <v>498.48</v>
       </c>
     </row>
     <row r="444" spans="1:2">
@@ -5526,7 +5526,7 @@
         <v>444</v>
       </c>
       <c r="B444">
-        <v>281.2</v>
+        <v>337.44</v>
       </c>
     </row>
     <row r="445" spans="1:2">
@@ -5534,7 +5534,7 @@
         <v>445</v>
       </c>
       <c r="B445">
-        <v>161.12</v>
+        <v>193.344</v>
       </c>
     </row>
     <row r="446" spans="1:2">
@@ -5542,7 +5542,7 @@
         <v>446</v>
       </c>
       <c r="B446">
-        <v>138.6</v>
+        <v>166.32</v>
       </c>
     </row>
     <row r="447" spans="1:2">
@@ -5550,7 +5550,7 @@
         <v>447</v>
       </c>
       <c r="B447">
-        <v>78.40000000000001</v>
+        <v>94.08</v>
       </c>
     </row>
     <row r="448" spans="1:2">
@@ -5558,7 +5558,7 @@
         <v>448</v>
       </c>
       <c r="B448">
-        <v>55.16</v>
+        <v>66.19200000000001</v>
       </c>
     </row>
     <row r="449" spans="1:2">
@@ -5566,7 +5566,7 @@
         <v>449</v>
       </c>
       <c r="B449">
-        <v>335.34</v>
+        <v>402.408</v>
       </c>
     </row>
     <row r="450" spans="1:2">
@@ -5574,7 +5574,7 @@
         <v>450</v>
       </c>
       <c r="B450">
-        <v>1.4</v>
+        <v>1.68</v>
       </c>
     </row>
     <row r="451" spans="1:2">
@@ -5582,7 +5582,7 @@
         <v>451</v>
       </c>
       <c r="B451">
-        <v>611.9400000000001</v>
+        <v>727.128</v>
       </c>
     </row>
     <row r="452" spans="1:2">
@@ -5590,7 +5590,7 @@
         <v>452</v>
       </c>
       <c r="B452">
-        <v>405.7199999999999</v>
+        <v>486.864</v>
       </c>
     </row>
     <row r="453" spans="1:2">
@@ -5598,7 +5598,7 @@
         <v>453</v>
       </c>
       <c r="B453">
-        <v>128.64</v>
+        <v>154.368</v>
       </c>
     </row>
     <row r="454" spans="1:2">
@@ -5606,7 +5606,7 @@
         <v>454</v>
       </c>
       <c r="B454">
-        <v>11.76</v>
+        <v>14.112</v>
       </c>
     </row>
     <row r="455" spans="1:2">
@@ -5614,7 +5614,7 @@
         <v>455</v>
       </c>
       <c r="B455">
-        <v>322.92</v>
+        <v>387.504</v>
       </c>
     </row>
     <row r="456" spans="1:2">
@@ -5622,7 +5622,7 @@
         <v>456</v>
       </c>
       <c r="B456">
-        <v>415.86</v>
+        <v>503.8319999999999</v>
       </c>
     </row>
     <row r="457" spans="1:2">
@@ -5630,7 +5630,7 @@
         <v>457</v>
       </c>
       <c r="B457">
-        <v>408.36</v>
+        <v>490.032</v>
       </c>
     </row>
     <row r="458" spans="1:2">
@@ -5638,7 +5638,7 @@
         <v>458</v>
       </c>
       <c r="B458">
-        <v>449.6</v>
+        <v>539.52</v>
       </c>
     </row>
     <row r="459" spans="1:2">
@@ -5646,7 +5646,7 @@
         <v>459</v>
       </c>
       <c r="B459">
-        <v>56.76</v>
+        <v>68.11199999999999</v>
       </c>
     </row>
     <row r="460" spans="1:2">
@@ -5654,7 +5654,7 @@
         <v>460</v>
       </c>
       <c r="B460">
-        <v>2.4</v>
+        <v>2.88</v>
       </c>
     </row>
     <row r="461" spans="1:2">
@@ -5662,7 +5662,7 @@
         <v>461</v>
       </c>
       <c r="B461">
-        <v>410.9999999999999</v>
+        <v>493.2</v>
       </c>
     </row>
     <row r="462" spans="1:2">
@@ -5670,7 +5670,7 @@
         <v>462</v>
       </c>
       <c r="B462">
-        <v>135.2</v>
+        <v>162.24</v>
       </c>
     </row>
     <row r="463" spans="1:2">
@@ -5678,7 +5678,7 @@
         <v>463</v>
       </c>
       <c r="B463">
-        <v>104.96</v>
+        <v>125.952</v>
       </c>
     </row>
     <row r="464" spans="1:2">
@@ -5686,7 +5686,7 @@
         <v>464</v>
       </c>
       <c r="B464">
-        <v>370.64</v>
+        <v>444.768</v>
       </c>
     </row>
     <row r="465" spans="1:2">
@@ -5694,7 +5694,7 @@
         <v>465</v>
       </c>
       <c r="B465">
-        <v>1.8</v>
+        <v>2.16</v>
       </c>
     </row>
     <row r="466" spans="1:2">
@@ -5702,7 +5702,7 @@
         <v>466</v>
       </c>
       <c r="B466">
-        <v>34.95999999999999</v>
+        <v>41.95199999999999</v>
       </c>
     </row>
     <row r="467" spans="1:2">
@@ -5710,7 +5710,7 @@
         <v>467</v>
       </c>
       <c r="B467">
-        <v>0.4</v>
+        <v>0.48</v>
       </c>
     </row>
     <row r="468" spans="1:2">
@@ -5718,7 +5718,7 @@
         <v>468</v>
       </c>
       <c r="B468">
-        <v>37.8</v>
+        <v>45.36</v>
       </c>
     </row>
     <row r="469" spans="1:2">
@@ -5726,7 +5726,7 @@
         <v>469</v>
       </c>
       <c r="B469">
-        <v>494</v>
+        <v>597.6</v>
       </c>
     </row>
     <row r="470" spans="1:2">
@@ -5734,7 +5734,7 @@
         <v>470</v>
       </c>
       <c r="B470">
-        <v>233.16</v>
+        <v>279.792</v>
       </c>
     </row>
     <row r="471" spans="1:2">
@@ -5742,7 +5742,7 @@
         <v>471</v>
       </c>
       <c r="B471">
-        <v>462</v>
+        <v>554.4</v>
       </c>
     </row>
     <row r="472" spans="1:2">
@@ -5750,7 +5750,7 @@
         <v>472</v>
       </c>
       <c r="B472">
-        <v>14.82</v>
+        <v>17.784</v>
       </c>
     </row>
     <row r="473" spans="1:2">
@@ -5758,7 +5758,7 @@
         <v>473</v>
       </c>
       <c r="B473">
-        <v>31.8</v>
+        <v>38.16</v>
       </c>
     </row>
     <row r="474" spans="1:2">
@@ -5766,7 +5766,7 @@
         <v>474</v>
       </c>
       <c r="B474">
-        <v>322.4</v>
+        <v>386.88</v>
       </c>
     </row>
     <row r="475" spans="1:2">
@@ -5774,7 +5774,7 @@
         <v>475</v>
       </c>
       <c r="B475">
-        <v>226.8</v>
+        <v>272.16</v>
       </c>
     </row>
     <row r="476" spans="1:2">
@@ -5782,7 +5782,7 @@
         <v>476</v>
       </c>
       <c r="B476">
-        <v>163.2</v>
+        <v>195.84</v>
       </c>
     </row>
     <row r="477" spans="1:2">
@@ -5790,7 +5790,7 @@
         <v>477</v>
       </c>
       <c r="B477">
-        <v>187.74</v>
+        <v>225.288</v>
       </c>
     </row>
     <row r="478" spans="1:2">
@@ -5798,7 +5798,7 @@
         <v>478</v>
       </c>
       <c r="B478">
-        <v>172.16</v>
+        <v>206.592</v>
       </c>
     </row>
     <row r="479" spans="1:2">
@@ -5806,7 +5806,7 @@
         <v>479</v>
       </c>
       <c r="B479">
-        <v>270.1</v>
+        <v>324.12</v>
       </c>
     </row>
     <row r="480" spans="1:2">
@@ -5814,7 +5814,7 @@
         <v>480</v>
       </c>
       <c r="B480">
-        <v>500.7799999999999</v>
+        <v>600.9359999999999</v>
       </c>
     </row>
     <row r="481" spans="1:2">
@@ -5822,7 +5822,7 @@
         <v>481</v>
       </c>
       <c r="B481">
-        <v>214.12</v>
+        <v>256.944</v>
       </c>
     </row>
     <row r="482" spans="1:2">
@@ -5830,7 +5830,7 @@
         <v>482</v>
       </c>
       <c r="B482">
-        <v>230.68</v>
+        <v>276.816</v>
       </c>
     </row>
     <row r="483" spans="1:2">
@@ -5838,7 +5838,7 @@
         <v>483</v>
       </c>
       <c r="B483">
-        <v>350.7599999999999</v>
+        <v>420.912</v>
       </c>
     </row>
     <row r="484" spans="1:2">
@@ -5846,7 +5846,7 @@
         <v>484</v>
       </c>
       <c r="B484">
-        <v>607.84</v>
+        <v>790.6080000000001</v>
       </c>
     </row>
     <row r="485" spans="1:2">
@@ -5854,7 +5854,7 @@
         <v>485</v>
       </c>
       <c r="B485">
-        <v>455.92</v>
+        <v>547.1039999999999</v>
       </c>
     </row>
     <row r="486" spans="1:2">
@@ -5862,7 +5862,7 @@
         <v>486</v>
       </c>
       <c r="B486">
-        <v>406.06</v>
+        <v>487.272</v>
       </c>
     </row>
     <row r="487" spans="1:2">
@@ -5870,7 +5870,7 @@
         <v>487</v>
       </c>
       <c r="B487">
-        <v>366.6</v>
+        <v>439.92</v>
       </c>
     </row>
     <row r="488" spans="1:2">
@@ -5878,7 +5878,7 @@
         <v>488</v>
       </c>
       <c r="B488">
-        <v>162.54</v>
+        <v>195.048</v>
       </c>
     </row>
     <row r="489" spans="1:2">
@@ -5886,7 +5886,7 @@
         <v>489</v>
       </c>
       <c r="B489">
-        <v>332.28</v>
+        <v>398.7359999999999</v>
       </c>
     </row>
     <row r="490" spans="1:2">
@@ -5894,7 +5894,7 @@
         <v>490</v>
       </c>
       <c r="B490">
-        <v>344.96</v>
+        <v>413.952</v>
       </c>
     </row>
     <row r="491" spans="1:2">
@@ -5902,7 +5902,7 @@
         <v>491</v>
       </c>
       <c r="B491">
-        <v>418.8799999999999</v>
+        <v>502.656</v>
       </c>
     </row>
     <row r="492" spans="1:2">
@@ -5910,7 +5910,7 @@
         <v>492</v>
       </c>
       <c r="B492">
-        <v>304</v>
+        <v>364.8</v>
       </c>
     </row>
     <row r="493" spans="1:2">
@@ -5918,7 +5918,7 @@
         <v>493</v>
       </c>
       <c r="B493">
-        <v>42.56</v>
+        <v>51.072</v>
       </c>
     </row>
     <row r="494" spans="1:2">
@@ -5926,7 +5926,7 @@
         <v>494</v>
       </c>
       <c r="B494">
-        <v>174.96</v>
+        <v>209.952</v>
       </c>
     </row>
     <row r="495" spans="1:2">
@@ -5934,7 +5934,7 @@
         <v>495</v>
       </c>
       <c r="B495">
-        <v>336.3</v>
+        <v>403.56</v>
       </c>
     </row>
     <row r="496" spans="1:2">
@@ -5942,7 +5942,7 @@
         <v>496</v>
       </c>
       <c r="B496">
-        <v>306.86</v>
+        <v>368.232</v>
       </c>
     </row>
     <row r="497" spans="1:2">
@@ -5950,7 +5950,7 @@
         <v>497</v>
       </c>
       <c r="B497">
-        <v>183.6</v>
+        <v>220.32</v>
       </c>
     </row>
     <row r="498" spans="1:2">
@@ -5958,7 +5958,7 @@
         <v>498</v>
       </c>
       <c r="B498">
-        <v>547.2</v>
+        <v>656.64</v>
       </c>
     </row>
     <row r="499" spans="1:2">
@@ -5966,7 +5966,7 @@
         <v>499</v>
       </c>
       <c r="B499">
-        <v>282.08</v>
+        <v>338.496</v>
       </c>
     </row>
     <row r="500" spans="1:2">
@@ -5974,7 +5974,7 @@
         <v>500</v>
       </c>
       <c r="B500">
-        <v>170.4</v>
+        <v>204.48</v>
       </c>
     </row>
     <row r="501" spans="1:2">
@@ -5982,7 +5982,7 @@
         <v>501</v>
       </c>
       <c r="B501">
-        <v>492</v>
+        <v>590.4</v>
       </c>
     </row>
     <row r="502" spans="1:2">
@@ -5990,7 +5990,7 @@
         <v>502</v>
       </c>
       <c r="B502">
-        <v>29.44</v>
+        <v>35.328</v>
       </c>
     </row>
     <row r="503" spans="1:2">
@@ -5998,7 +5998,7 @@
         <v>503</v>
       </c>
       <c r="B503">
-        <v>5.399999999999999</v>
+        <v>6.48</v>
       </c>
     </row>
     <row r="504" spans="1:2">
@@ -6006,7 +6006,7 @@
         <v>504</v>
       </c>
       <c r="B504">
-        <v>429</v>
+        <v>514.8</v>
       </c>
     </row>
     <row r="505" spans="1:2">
@@ -6014,7 +6014,7 @@
         <v>505</v>
       </c>
       <c r="B505">
-        <v>45.56</v>
+        <v>54.672</v>
       </c>
     </row>
     <row r="506" spans="1:2">
@@ -6022,7 +6022,7 @@
         <v>506</v>
       </c>
       <c r="B506">
-        <v>24</v>
+        <v>28.8</v>
       </c>
     </row>
     <row r="507" spans="1:2">
@@ -6030,7 +6030,7 @@
         <v>507</v>
       </c>
       <c r="B507">
-        <v>47.52</v>
+        <v>57.02399999999999</v>
       </c>
     </row>
     <row r="508" spans="1:2">
@@ -6038,7 +6038,7 @@
         <v>508</v>
       </c>
       <c r="B508">
-        <v>200.02</v>
+        <v>240.024</v>
       </c>
     </row>
     <row r="509" spans="1:2">
@@ -6046,7 +6046,7 @@
         <v>509</v>
       </c>
       <c r="B509">
-        <v>606.4</v>
+        <v>788.88</v>
       </c>
     </row>
     <row r="510" spans="1:2">
@@ -6054,7 +6054,7 @@
         <v>510</v>
       </c>
       <c r="B510">
-        <v>41.7</v>
+        <v>50.04</v>
       </c>
     </row>
     <row r="511" spans="1:2">
@@ -6062,7 +6062,7 @@
         <v>511</v>
       </c>
       <c r="B511">
-        <v>27.88</v>
+        <v>33.456</v>
       </c>
     </row>
     <row r="512" spans="1:2">
@@ -6070,7 +6070,7 @@
         <v>512</v>
       </c>
       <c r="B512">
-        <v>15.96</v>
+        <v>19.152</v>
       </c>
     </row>
     <row r="513" spans="1:2">
@@ -6078,7 +6078,7 @@
         <v>513</v>
       </c>
       <c r="B513">
-        <v>36.16</v>
+        <v>43.392</v>
       </c>
     </row>
     <row r="514" spans="1:2">
@@ -6086,7 +6086,7 @@
         <v>514</v>
       </c>
       <c r="B514">
-        <v>273.24</v>
+        <v>327.888</v>
       </c>
     </row>
     <row r="515" spans="1:2">
@@ -6094,7 +6094,7 @@
         <v>515</v>
       </c>
       <c r="B515">
-        <v>595.3199999999999</v>
+        <v>714.3839999999999</v>
       </c>
     </row>
     <row r="516" spans="1:2">
@@ -6102,7 +6102,7 @@
         <v>516</v>
       </c>
       <c r="B516">
-        <v>6.6</v>
+        <v>7.92</v>
       </c>
     </row>
     <row r="517" spans="1:2">
@@ -6110,7 +6110,7 @@
         <v>517</v>
       </c>
       <c r="B517">
-        <v>30.4</v>
+        <v>36.48</v>
       </c>
     </row>
     <row r="518" spans="1:2">
@@ -6118,7 +6118,7 @@
         <v>518</v>
       </c>
       <c r="B518">
-        <v>14</v>
+        <v>16.8</v>
       </c>
     </row>
     <row r="519" spans="1:2">
@@ -6126,7 +6126,7 @@
         <v>519</v>
       </c>
       <c r="B519">
-        <v>141.36</v>
+        <v>169.632</v>
       </c>
     </row>
     <row r="520" spans="1:2">
@@ -6134,7 +6134,7 @@
         <v>520</v>
       </c>
       <c r="B520">
-        <v>1.8</v>
+        <v>2.16</v>
       </c>
     </row>
     <row r="521" spans="1:2">
@@ -6142,7 +6142,7 @@
         <v>521</v>
       </c>
       <c r="B521">
-        <v>878.2399999999999</v>
+        <v>831.8879999999999</v>
       </c>
     </row>
     <row r="522" spans="1:2">
@@ -6150,7 +6150,7 @@
         <v>522</v>
       </c>
       <c r="B522">
-        <v>400.92</v>
+        <v>481.104</v>
       </c>
     </row>
     <row r="523" spans="1:2">
@@ -6158,7 +6158,7 @@
         <v>523</v>
       </c>
       <c r="B523">
-        <v>2.22</v>
+        <v>2.664</v>
       </c>
     </row>
     <row r="524" spans="1:2">
@@ -6166,7 +6166,7 @@
         <v>524</v>
       </c>
       <c r="B524">
-        <v>61.31999999999999</v>
+        <v>73.58399999999999</v>
       </c>
     </row>
     <row r="525" spans="1:2">
@@ -6174,7 +6174,7 @@
         <v>525</v>
       </c>
       <c r="B525">
-        <v>14.08</v>
+        <v>16.896</v>
       </c>
     </row>
     <row r="526" spans="1:2">
@@ -6182,7 +6182,7 @@
         <v>526</v>
       </c>
       <c r="B526">
-        <v>54.90000000000001</v>
+        <v>65.88</v>
       </c>
     </row>
     <row r="527" spans="1:2">
@@ -6190,7 +6190,7 @@
         <v>527</v>
       </c>
       <c r="B527">
-        <v>335.92</v>
+        <v>403.104</v>
       </c>
     </row>
     <row r="528" spans="1:2">
@@ -6198,7 +6198,7 @@
         <v>528</v>
       </c>
       <c r="B528">
-        <v>7.74</v>
+        <v>9.287999999999998</v>
       </c>
     </row>
     <row r="529" spans="1:2">
@@ -6206,7 +6206,7 @@
         <v>529</v>
       </c>
       <c r="B529">
-        <v>3.799999999999999</v>
+        <v>4.56</v>
       </c>
     </row>
     <row r="530" spans="1:2">
@@ -6214,7 +6214,7 @@
         <v>530</v>
       </c>
       <c r="B530">
-        <v>76.16</v>
+        <v>91.392</v>
       </c>
     </row>
     <row r="531" spans="1:2">
@@ -6222,7 +6222,7 @@
         <v>531</v>
       </c>
       <c r="B531">
-        <v>287.04</v>
+        <v>344.448</v>
       </c>
     </row>
     <row r="532" spans="1:2">
@@ -6230,7 +6230,7 @@
         <v>532</v>
       </c>
       <c r="B532">
-        <v>46.86</v>
+        <v>56.23199999999999</v>
       </c>
     </row>
     <row r="533" spans="1:2">
@@ -6238,7 +6238,7 @@
         <v>533</v>
       </c>
       <c r="B533">
-        <v>12.24</v>
+        <v>14.688</v>
       </c>
     </row>
     <row r="534" spans="1:2">
@@ -6246,7 +6246,7 @@
         <v>534</v>
       </c>
       <c r="B534">
-        <v>111.3</v>
+        <v>133.56</v>
       </c>
     </row>
     <row r="535" spans="1:2">
@@ -6254,7 +6254,7 @@
         <v>535</v>
       </c>
       <c r="B535">
-        <v>278.4</v>
+        <v>334.08</v>
       </c>
     </row>
     <row r="536" spans="1:2">
@@ -6262,7 +6262,7 @@
         <v>536</v>
       </c>
       <c r="B536">
-        <v>521.64</v>
+        <v>625.9680000000001</v>
       </c>
     </row>
     <row r="537" spans="1:2">
@@ -6270,7 +6270,7 @@
         <v>537</v>
       </c>
       <c r="B537">
-        <v>125.4</v>
+        <v>150.48</v>
       </c>
     </row>
     <row r="538" spans="1:2">
@@ -6278,7 +6278,7 @@
         <v>538</v>
       </c>
       <c r="B538">
-        <v>221.76</v>
+        <v>266.112</v>
       </c>
     </row>
     <row r="539" spans="1:2">
@@ -6286,7 +6286,7 @@
         <v>539</v>
       </c>
       <c r="B539">
-        <v>165.24</v>
+        <v>198.288</v>
       </c>
     </row>
     <row r="540" spans="1:2">
@@ -6294,7 +6294,7 @@
         <v>540</v>
       </c>
       <c r="B540">
-        <v>42.88</v>
+        <v>51.456</v>
       </c>
     </row>
     <row r="541" spans="1:2">
@@ -6302,7 +6302,7 @@
         <v>541</v>
       </c>
       <c r="B541">
-        <v>81.7</v>
+        <v>98.03999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>